<commit_message>
Added updated GUI based system
</commit_message>
<xml_diff>
--- a/example/trajectories (version 1).xlsb_scott_processed.xlsx
+++ b/example/trajectories (version 1).xlsb_scott_processed.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Scott Proccesed Flies" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Scott Processed Flies" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -517,12 +517,8 @@
       <c r="B2" t="n">
         <v>805.832</v>
       </c>
-      <c r="C2" t="n">
-        <v>585.27</v>
-      </c>
-      <c r="D2" t="n">
-        <v>935.0890000000001</v>
-      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="n">
         <v>494.608</v>
       </c>
@@ -531,12 +527,8 @@
       </c>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
-      <c r="I2" t="n">
-        <v>643.034</v>
-      </c>
-      <c r="J2" t="n">
-        <v>943.548</v>
-      </c>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="n">
@@ -550,30 +542,26 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="n">
+      <c r="A3" t="n">
         <v>494.613</v>
       </c>
-      <c r="D3" t="n">
+      <c r="B3" t="n">
         <v>761.807</v>
       </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="n">
+        <v>555.4109999999999</v>
+      </c>
+      <c r="F3" t="n">
+        <v>802.888</v>
+      </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
-      <c r="I3" t="n">
-        <v>643.337</v>
-      </c>
-      <c r="J3" t="n">
-        <v>943.734</v>
-      </c>
-      <c r="K3" t="n">
-        <v>555.4109999999999</v>
-      </c>
-      <c r="L3" t="n">
-        <v>802.888</v>
-      </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
       <c r="M3" t="n">
         <v>551.141</v>
       </c>
@@ -585,30 +573,26 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr"/>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="n">
+      <c r="A4" t="n">
         <v>494.658</v>
       </c>
-      <c r="D4" t="n">
+      <c r="B4" t="n">
         <v>761.876</v>
       </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="n">
+        <v>559.48</v>
+      </c>
+      <c r="F4" t="n">
+        <v>804.409</v>
+      </c>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
-      <c r="I4" t="n">
-        <v>643.535</v>
-      </c>
-      <c r="J4" t="n">
-        <v>943.758</v>
-      </c>
-      <c r="K4" t="n">
-        <v>559.48</v>
-      </c>
-      <c r="L4" t="n">
-        <v>804.409</v>
-      </c>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
       <c r="M4" t="n">
         <v>553.261</v>
       </c>
@@ -621,31 +605,27 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
+        <v>494.648</v>
+      </c>
+      <c r="B5" t="n">
+        <v>761.987</v>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="n">
         <v>563.602</v>
       </c>
-      <c r="B5" t="n">
+      <c r="F5" t="n">
         <v>806.732</v>
       </c>
-      <c r="C5" t="n">
-        <v>494.648</v>
-      </c>
-      <c r="D5" t="n">
-        <v>761.987</v>
-      </c>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
       <c r="G5" t="n">
         <v>625.273</v>
       </c>
       <c r="H5" t="n">
         <v>848.1660000000001</v>
       </c>
-      <c r="I5" t="n">
-        <v>645.249</v>
-      </c>
-      <c r="J5" t="n">
-        <v>943.6420000000001</v>
-      </c>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="n">
@@ -660,31 +640,27 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
+        <v>494.538</v>
+      </c>
+      <c r="B6" t="n">
+        <v>761.857</v>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="n">
         <v>565.663</v>
       </c>
-      <c r="B6" t="n">
+      <c r="F6" t="n">
         <v>805.073</v>
       </c>
-      <c r="C6" t="n">
-        <v>494.538</v>
-      </c>
-      <c r="D6" t="n">
-        <v>761.857</v>
-      </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
       <c r="G6" t="n">
         <v>624.528</v>
       </c>
       <c r="H6" t="n">
         <v>846.842</v>
       </c>
-      <c r="I6" t="n">
-        <v>647.6</v>
-      </c>
-      <c r="J6" t="n">
-        <v>935.33</v>
-      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
       <c r="K6" t="n">
         <v>623.399</v>
       </c>
@@ -703,19 +679,19 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
+        <v>494.629</v>
+      </c>
+      <c r="B7" t="n">
+        <v>761.856</v>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="n">
         <v>566.543</v>
       </c>
-      <c r="B7" t="n">
+      <c r="F7" t="n">
         <v>804.456</v>
       </c>
-      <c r="C7" t="n">
-        <v>494.629</v>
-      </c>
-      <c r="D7" t="n">
-        <v>761.856</v>
-      </c>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
       <c r="G7" t="n">
         <v>628.2859999999999</v>
       </c>
@@ -742,19 +718,19 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
+        <v>494.716</v>
+      </c>
+      <c r="B8" t="n">
+        <v>761.899</v>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="n">
         <v>566.0410000000001</v>
       </c>
-      <c r="B8" t="n">
+      <c r="F8" t="n">
         <v>804.765</v>
       </c>
-      <c r="C8" t="n">
-        <v>494.716</v>
-      </c>
-      <c r="D8" t="n">
-        <v>761.899</v>
-      </c>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
       <c r="G8" t="n">
         <v>633.026</v>
       </c>
@@ -781,31 +757,27 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
+        <v>494.629</v>
+      </c>
+      <c r="B9" t="n">
+        <v>761.783</v>
+      </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="n">
         <v>572.598</v>
       </c>
-      <c r="B9" t="n">
+      <c r="F9" t="n">
         <v>803.104</v>
       </c>
-      <c r="C9" t="n">
-        <v>494.629</v>
-      </c>
-      <c r="D9" t="n">
-        <v>761.783</v>
-      </c>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
       <c r="G9" t="n">
         <v>635.756</v>
       </c>
       <c r="H9" t="n">
         <v>825.338</v>
       </c>
-      <c r="I9" t="n">
-        <v>627.465</v>
-      </c>
-      <c r="J9" t="n">
-        <v>889.134</v>
-      </c>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
       <c r="K9" t="n">
         <v>639.441</v>
       </c>
@@ -824,31 +796,27 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
+        <v>494.708</v>
+      </c>
+      <c r="B10" t="n">
+        <v>761.694</v>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="n">
         <v>576.151</v>
       </c>
-      <c r="B10" t="n">
+      <c r="F10" t="n">
         <v>804.71</v>
       </c>
-      <c r="C10" t="n">
-        <v>494.708</v>
-      </c>
-      <c r="D10" t="n">
-        <v>761.694</v>
-      </c>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
       <c r="G10" t="n">
         <v>637.342</v>
       </c>
       <c r="H10" t="n">
         <v>814.035</v>
       </c>
-      <c r="I10" t="n">
-        <v>624.299</v>
-      </c>
-      <c r="J10" t="n">
-        <v>878.241</v>
-      </c>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
       <c r="K10" t="n">
         <v>635.086</v>
       </c>
@@ -867,31 +835,27 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
+        <v>494.599</v>
+      </c>
+      <c r="B11" t="n">
+        <v>761.428</v>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="n">
         <v>579.7619999999999</v>
       </c>
-      <c r="B11" t="n">
+      <c r="F11" t="n">
         <v>799.8049999999999</v>
       </c>
-      <c r="C11" t="n">
-        <v>494.599</v>
-      </c>
-      <c r="D11" t="n">
-        <v>761.428</v>
-      </c>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
       <c r="G11" t="n">
         <v>639.996</v>
       </c>
       <c r="H11" t="n">
         <v>806.606</v>
       </c>
-      <c r="I11" t="n">
-        <v>620.269</v>
-      </c>
-      <c r="J11" t="n">
-        <v>869.612</v>
-      </c>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
       <c r="K11" t="n">
         <v>635.869</v>
       </c>
@@ -910,31 +874,27 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
+        <v>494.57</v>
+      </c>
+      <c r="B12" t="n">
+        <v>760.157</v>
+      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="n">
         <v>578.045</v>
       </c>
-      <c r="B12" t="n">
+      <c r="F12" t="n">
         <v>798.519</v>
       </c>
-      <c r="C12" t="n">
-        <v>494.57</v>
-      </c>
-      <c r="D12" t="n">
-        <v>760.157</v>
-      </c>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
       <c r="G12" t="n">
         <v>641.389</v>
       </c>
       <c r="H12" t="n">
         <v>794.672</v>
       </c>
-      <c r="I12" t="n">
-        <v>618</v>
-      </c>
-      <c r="J12" t="n">
-        <v>858.588</v>
-      </c>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="n">
@@ -964,12 +924,8 @@
       </c>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
-      <c r="I13" t="n">
-        <v>617.011</v>
-      </c>
-      <c r="J13" t="n">
-        <v>850.5069999999999</v>
-      </c>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
       <c r="K13" t="n">
         <v>638.183</v>
       </c>
@@ -993,12 +949,8 @@
       <c r="B14" t="n">
         <v>795.379</v>
       </c>
-      <c r="C14" t="n">
-        <v>643.947</v>
-      </c>
-      <c r="D14" t="n">
-        <v>777.96</v>
-      </c>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
       <c r="E14" t="n">
         <v>492.054</v>
       </c>
@@ -1007,12 +959,8 @@
       </c>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
-      <c r="I14" t="n">
-        <v>614.441</v>
-      </c>
-      <c r="J14" t="n">
-        <v>839.875</v>
-      </c>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
       <c r="K14" t="n">
         <v>638.104</v>
       </c>
@@ -1036,12 +984,8 @@
       <c r="B15" t="n">
         <v>791.883</v>
       </c>
-      <c r="C15" t="n">
-        <v>644.499</v>
-      </c>
-      <c r="D15" t="n">
-        <v>772.2329999999999</v>
-      </c>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
       <c r="E15" t="n">
         <v>492.432</v>
       </c>
@@ -1054,12 +998,8 @@
       <c r="H15" t="n">
         <v>891.001</v>
       </c>
-      <c r="I15" t="n">
-        <v>613.8150000000001</v>
-      </c>
-      <c r="J15" t="n">
-        <v>829.878</v>
-      </c>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
       <c r="K15" t="n">
         <v>638.328</v>
       </c>
@@ -1083,12 +1023,8 @@
       <c r="B16" t="n">
         <v>789.518</v>
       </c>
-      <c r="C16" t="n">
-        <v>644.684</v>
-      </c>
-      <c r="D16" t="n">
-        <v>767.98</v>
-      </c>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
       <c r="E16" t="n">
         <v>492.738</v>
       </c>
@@ -1097,12 +1033,8 @@
       </c>
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr"/>
-      <c r="I16" t="n">
-        <v>614.066</v>
-      </c>
-      <c r="J16" t="n">
-        <v>819.958</v>
-      </c>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
       <c r="K16" t="n">
         <v>638.761</v>
       </c>
@@ -1126,12 +1058,8 @@
       <c r="B17" t="n">
         <v>789.396</v>
       </c>
-      <c r="C17" t="n">
-        <v>646.369</v>
-      </c>
-      <c r="D17" t="n">
-        <v>759.508</v>
-      </c>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
       <c r="E17" t="n">
         <v>491.295</v>
       </c>
@@ -1140,12 +1068,8 @@
       </c>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr"/>
-      <c r="I17" t="n">
-        <v>613.424</v>
-      </c>
-      <c r="J17" t="n">
-        <v>813.674</v>
-      </c>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
       <c r="K17" t="n">
         <v>634.871</v>
       </c>
@@ -1169,12 +1093,8 @@
       <c r="B18" t="n">
         <v>789.0650000000001</v>
       </c>
-      <c r="C18" t="n">
-        <v>646.84</v>
-      </c>
-      <c r="D18" t="n">
-        <v>748.881</v>
-      </c>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
       <c r="E18" t="n">
         <v>489.725</v>
       </c>
@@ -1183,12 +1103,8 @@
       </c>
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr"/>
-      <c r="I18" t="n">
-        <v>613.191</v>
-      </c>
-      <c r="J18" t="n">
-        <v>812.523</v>
-      </c>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
       <c r="K18" t="n">
         <v>639.7670000000001</v>
       </c>
@@ -1212,12 +1128,8 @@
       <c r="B19" t="n">
         <v>788.168</v>
       </c>
-      <c r="C19" t="n">
-        <v>647.783</v>
-      </c>
-      <c r="D19" t="n">
-        <v>740.707</v>
-      </c>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr"/>
       <c r="E19" t="n">
         <v>487.656</v>
       </c>
@@ -1226,12 +1138,8 @@
       </c>
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr"/>
-      <c r="I19" t="n">
-        <v>613.226</v>
-      </c>
-      <c r="J19" t="n">
-        <v>813.096</v>
-      </c>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr"/>
       <c r="K19" t="n">
         <v>643.254</v>
       </c>
@@ -1255,12 +1163,8 @@
       <c r="B20" t="n">
         <v>789.211</v>
       </c>
-      <c r="C20" t="n">
-        <v>648.28</v>
-      </c>
-      <c r="D20" t="n">
-        <v>730.66</v>
-      </c>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr"/>
       <c r="E20" t="n">
         <v>485.788</v>
       </c>
@@ -1273,12 +1177,8 @@
       <c r="H20" t="n">
         <v>939.46</v>
       </c>
-      <c r="I20" t="n">
-        <v>613.247</v>
-      </c>
-      <c r="J20" t="n">
-        <v>812.801</v>
-      </c>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr"/>
       <c r="K20" t="n">
         <v>647.1420000000001</v>
       </c>
@@ -1302,12 +1202,8 @@
       <c r="B21" t="n">
         <v>789.325</v>
       </c>
-      <c r="C21" t="n">
-        <v>649.321</v>
-      </c>
-      <c r="D21" t="n">
-        <v>721.404</v>
-      </c>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr"/>
       <c r="E21" t="n">
         <v>485.059</v>
       </c>
@@ -1320,12 +1216,8 @@
       <c r="H21" t="n">
         <v>939.359</v>
       </c>
-      <c r="I21" t="n">
-        <v>613.322</v>
-      </c>
-      <c r="J21" t="n">
-        <v>812.913</v>
-      </c>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr"/>
       <c r="K21" t="n">
         <v>649.633</v>
       </c>
@@ -1349,12 +1241,8 @@
       <c r="B22" t="n">
         <v>789.5940000000001</v>
       </c>
-      <c r="C22" t="n">
-        <v>649.546</v>
-      </c>
-      <c r="D22" t="n">
-        <v>710.3200000000001</v>
-      </c>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr"/>
       <c r="E22" t="n">
         <v>482.482</v>
       </c>
@@ -1367,12 +1255,8 @@
       <c r="H22" t="n">
         <v>937.139</v>
       </c>
-      <c r="I22" t="n">
-        <v>613.271</v>
-      </c>
-      <c r="J22" t="n">
-        <v>813.042</v>
-      </c>
+      <c r="I22" t="inlineStr"/>
+      <c r="J22" t="inlineStr"/>
       <c r="K22" t="n">
         <v>650.856</v>
       </c>
@@ -1396,12 +1280,8 @@
       <c r="B23" t="n">
         <v>787.777</v>
       </c>
-      <c r="C23" t="n">
-        <v>649.55</v>
-      </c>
-      <c r="D23" t="n">
-        <v>701.163</v>
-      </c>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr"/>
       <c r="E23" t="n">
         <v>479.402</v>
       </c>
@@ -1414,12 +1294,8 @@
       <c r="H23" t="n">
         <v>933.8049999999999</v>
       </c>
-      <c r="I23" t="n">
-        <v>613.274</v>
-      </c>
-      <c r="J23" t="n">
-        <v>812.736</v>
-      </c>
+      <c r="I23" t="inlineStr"/>
+      <c r="J23" t="inlineStr"/>
       <c r="K23" t="n">
         <v>650.611</v>
       </c>
@@ -1443,12 +1319,8 @@
       <c r="B24" t="n">
         <v>785.86</v>
       </c>
-      <c r="C24" t="n">
-        <v>649.869</v>
-      </c>
-      <c r="D24" t="n">
-        <v>692.172</v>
-      </c>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr"/>
       <c r="E24" t="n">
         <v>477.597</v>
       </c>
@@ -1461,12 +1333,8 @@
       <c r="H24" t="n">
         <v>929.795</v>
       </c>
-      <c r="I24" t="n">
-        <v>613.266</v>
-      </c>
-      <c r="J24" t="n">
-        <v>813.265</v>
-      </c>
+      <c r="I24" t="inlineStr"/>
+      <c r="J24" t="inlineStr"/>
       <c r="K24" t="n">
         <v>649.324</v>
       </c>
@@ -1490,12 +1358,8 @@
       <c r="B25" t="n">
         <v>782.9589999999999</v>
       </c>
-      <c r="C25" t="n">
-        <v>650.4829999999999</v>
-      </c>
-      <c r="D25" t="n">
-        <v>681.29</v>
-      </c>
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr"/>
       <c r="E25" t="n">
         <v>475.084</v>
       </c>
@@ -1508,12 +1372,8 @@
       <c r="H25" t="n">
         <v>922.535</v>
       </c>
-      <c r="I25" t="n">
-        <v>613.296</v>
-      </c>
-      <c r="J25" t="n">
-        <v>812.997</v>
-      </c>
+      <c r="I25" t="inlineStr"/>
+      <c r="J25" t="inlineStr"/>
       <c r="K25" t="n">
         <v>648.41</v>
       </c>
@@ -1537,12 +1397,8 @@
       <c r="B26" t="n">
         <v>782.737</v>
       </c>
-      <c r="C26" t="n">
-        <v>650.326</v>
-      </c>
-      <c r="D26" t="n">
-        <v>670.785</v>
-      </c>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="inlineStr"/>
       <c r="E26" t="n">
         <v>473.496</v>
       </c>
@@ -1555,12 +1411,8 @@
       <c r="H26" t="n">
         <v>915.9640000000001</v>
       </c>
-      <c r="I26" t="n">
-        <v>613.3680000000001</v>
-      </c>
-      <c r="J26" t="n">
-        <v>813.33</v>
-      </c>
+      <c r="I26" t="inlineStr"/>
+      <c r="J26" t="inlineStr"/>
       <c r="K26" t="n">
         <v>646.629</v>
       </c>
@@ -1584,12 +1436,8 @@
       <c r="B27" t="n">
         <v>782.731</v>
       </c>
-      <c r="C27" t="n">
-        <v>649.706</v>
-      </c>
-      <c r="D27" t="n">
-        <v>660.157</v>
-      </c>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr"/>
       <c r="E27" t="n">
         <v>473.508</v>
       </c>
@@ -1602,12 +1450,8 @@
       <c r="H27" t="n">
         <v>911.745</v>
       </c>
-      <c r="I27" t="n">
-        <v>613.33</v>
-      </c>
-      <c r="J27" t="n">
-        <v>813.664</v>
-      </c>
+      <c r="I27" t="inlineStr"/>
+      <c r="J27" t="inlineStr"/>
       <c r="K27" t="n">
         <v>646.952</v>
       </c>
@@ -1631,12 +1475,8 @@
       <c r="B28" t="n">
         <v>782.655</v>
       </c>
-      <c r="C28" t="n">
-        <v>648.961</v>
-      </c>
-      <c r="D28" t="n">
-        <v>652.098</v>
-      </c>
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr"/>
       <c r="E28" t="n">
         <v>472.824</v>
       </c>
@@ -1674,12 +1514,8 @@
       <c r="B29" t="n">
         <v>782.5410000000001</v>
       </c>
-      <c r="C29" t="n">
-        <v>649.6180000000001</v>
-      </c>
-      <c r="D29" t="n">
-        <v>643.117</v>
-      </c>
+      <c r="C29" t="inlineStr"/>
+      <c r="D29" t="inlineStr"/>
       <c r="E29" t="n">
         <v>472.571</v>
       </c>
@@ -1692,12 +1528,8 @@
       <c r="H29" t="n">
         <v>902.063</v>
       </c>
-      <c r="I29" t="n">
-        <v>610.64</v>
-      </c>
-      <c r="J29" t="n">
-        <v>818.3099999999999</v>
-      </c>
+      <c r="I29" t="inlineStr"/>
+      <c r="J29" t="inlineStr"/>
       <c r="K29" t="n">
         <v>647.7619999999999</v>
       </c>
@@ -1721,12 +1553,8 @@
       <c r="B30" t="n">
         <v>782.745</v>
       </c>
-      <c r="C30" t="n">
-        <v>649.7089999999999</v>
-      </c>
-      <c r="D30" t="n">
-        <v>633.092</v>
-      </c>
+      <c r="C30" t="inlineStr"/>
+      <c r="D30" t="inlineStr"/>
       <c r="E30" t="n">
         <v>471.836</v>
       </c>
@@ -1739,12 +1567,8 @@
       <c r="H30" t="n">
         <v>896.6900000000001</v>
       </c>
-      <c r="I30" t="n">
-        <v>607.595</v>
-      </c>
-      <c r="J30" t="n">
-        <v>822.446</v>
-      </c>
+      <c r="I30" t="inlineStr"/>
+      <c r="J30" t="inlineStr"/>
       <c r="K30" t="n">
         <v>647.908</v>
       </c>
@@ -1768,12 +1592,8 @@
       <c r="B31" t="n">
         <v>782.426</v>
       </c>
-      <c r="C31" t="n">
-        <v>649.207</v>
-      </c>
-      <c r="D31" t="n">
-        <v>623.86</v>
-      </c>
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="inlineStr"/>
       <c r="E31" t="n">
         <v>471.676</v>
       </c>
@@ -1786,12 +1606,8 @@
       <c r="H31" t="n">
         <v>888.45</v>
       </c>
-      <c r="I31" t="n">
-        <v>603.74</v>
-      </c>
-      <c r="J31" t="n">
-        <v>820.4450000000001</v>
-      </c>
+      <c r="I31" t="inlineStr"/>
+      <c r="J31" t="inlineStr"/>
       <c r="K31" t="n">
         <v>648.5650000000001</v>
       </c>
@@ -1815,12 +1631,8 @@
       <c r="B32" t="n">
         <v>782.918</v>
       </c>
-      <c r="C32" t="n">
-        <v>648.511</v>
-      </c>
-      <c r="D32" t="n">
-        <v>615.028</v>
-      </c>
+      <c r="C32" t="inlineStr"/>
+      <c r="D32" t="inlineStr"/>
       <c r="E32" t="n">
         <v>471.427</v>
       </c>
@@ -1833,12 +1645,8 @@
       <c r="H32" t="n">
         <v>880.811</v>
       </c>
-      <c r="I32" t="n">
-        <v>598.62</v>
-      </c>
-      <c r="J32" t="n">
-        <v>818.973</v>
-      </c>
+      <c r="I32" t="inlineStr"/>
+      <c r="J32" t="inlineStr"/>
       <c r="K32" t="n">
         <v>648.128</v>
       </c>
@@ -1862,12 +1670,8 @@
       <c r="B33" t="n">
         <v>783.086</v>
       </c>
-      <c r="C33" t="n">
-        <v>648.578</v>
-      </c>
-      <c r="D33" t="n">
-        <v>605.297</v>
-      </c>
+      <c r="C33" t="inlineStr"/>
+      <c r="D33" t="inlineStr"/>
       <c r="E33" t="n">
         <v>470.555</v>
       </c>
@@ -1880,12 +1684,8 @@
       <c r="H33" t="n">
         <v>873.698</v>
       </c>
-      <c r="I33" t="n">
-        <v>597.213</v>
-      </c>
-      <c r="J33" t="n">
-        <v>817.668</v>
-      </c>
+      <c r="I33" t="inlineStr"/>
+      <c r="J33" t="inlineStr"/>
       <c r="K33" t="n">
         <v>648.821</v>
       </c>
@@ -1909,12 +1709,8 @@
       <c r="B34" t="n">
         <v>784.828</v>
       </c>
-      <c r="C34" t="n">
-        <v>648.466</v>
-      </c>
-      <c r="D34" t="n">
-        <v>599.0599999999999</v>
-      </c>
+      <c r="C34" t="inlineStr"/>
+      <c r="D34" t="inlineStr"/>
       <c r="E34" t="n">
         <v>469.41</v>
       </c>
@@ -1927,12 +1723,8 @@
       <c r="H34" t="n">
         <v>863.822</v>
       </c>
-      <c r="I34" t="n">
-        <v>594.981</v>
-      </c>
-      <c r="J34" t="n">
-        <v>815.751</v>
-      </c>
+      <c r="I34" t="inlineStr"/>
+      <c r="J34" t="inlineStr"/>
       <c r="K34" t="n">
         <v>648.574</v>
       </c>
@@ -1956,12 +1748,8 @@
       <c r="B35" t="n">
         <v>787.294</v>
       </c>
-      <c r="C35" t="n">
-        <v>647.016</v>
-      </c>
-      <c r="D35" t="n">
-        <v>590.591</v>
-      </c>
+      <c r="C35" t="inlineStr"/>
+      <c r="D35" t="inlineStr"/>
       <c r="E35" t="n">
         <v>469.196</v>
       </c>
@@ -1974,12 +1762,8 @@
       <c r="H35" t="n">
         <v>853.3440000000001</v>
       </c>
-      <c r="I35" t="n">
-        <v>588.158</v>
-      </c>
-      <c r="J35" t="n">
-        <v>812.866</v>
-      </c>
+      <c r="I35" t="inlineStr"/>
+      <c r="J35" t="inlineStr"/>
       <c r="K35" t="n">
         <v>648.951</v>
       </c>
@@ -2003,12 +1787,8 @@
       <c r="B36" t="n">
         <v>789.539</v>
       </c>
-      <c r="C36" t="n">
-        <v>646.946</v>
-      </c>
-      <c r="D36" t="n">
-        <v>581.0549999999999</v>
-      </c>
+      <c r="C36" t="inlineStr"/>
+      <c r="D36" t="inlineStr"/>
       <c r="E36" t="n">
         <v>469.276</v>
       </c>
@@ -2021,12 +1801,8 @@
       <c r="H36" t="n">
         <v>841.375</v>
       </c>
-      <c r="I36" t="n">
-        <v>581.597</v>
-      </c>
-      <c r="J36" t="n">
-        <v>808.188</v>
-      </c>
+      <c r="I36" t="inlineStr"/>
+      <c r="J36" t="inlineStr"/>
       <c r="K36" t="n">
         <v>648.967</v>
       </c>
@@ -2050,12 +1826,8 @@
       <c r="B37" t="n">
         <v>790.857</v>
       </c>
-      <c r="C37" t="n">
-        <v>646.5309999999999</v>
-      </c>
-      <c r="D37" t="n">
-        <v>573.3869999999999</v>
-      </c>
+      <c r="C37" t="inlineStr"/>
+      <c r="D37" t="inlineStr"/>
       <c r="E37" t="n">
         <v>469.295</v>
       </c>
@@ -2068,12 +1840,8 @@
       <c r="H37" t="n">
         <v>833.115</v>
       </c>
-      <c r="I37" t="n">
-        <v>571.967</v>
-      </c>
-      <c r="J37" t="n">
-        <v>801.592</v>
-      </c>
+      <c r="I37" t="inlineStr"/>
+      <c r="J37" t="inlineStr"/>
       <c r="K37" t="n">
         <v>648.259</v>
       </c>
@@ -2097,12 +1865,8 @@
       <c r="B38" t="n">
         <v>794.244</v>
       </c>
-      <c r="C38" t="n">
-        <v>646.759</v>
-      </c>
-      <c r="D38" t="n">
-        <v>567.487</v>
-      </c>
+      <c r="C38" t="inlineStr"/>
+      <c r="D38" t="inlineStr"/>
       <c r="E38" t="n">
         <v>469.167</v>
       </c>
@@ -2115,12 +1879,8 @@
       <c r="H38" t="n">
         <v>824.422</v>
       </c>
-      <c r="I38" t="n">
-        <v>565.222</v>
-      </c>
-      <c r="J38" t="n">
-        <v>797.515</v>
-      </c>
+      <c r="I38" t="inlineStr"/>
+      <c r="J38" t="inlineStr"/>
       <c r="K38" t="n">
         <v>649.654</v>
       </c>
@@ -2144,12 +1904,8 @@
       <c r="B39" t="n">
         <v>795.395</v>
       </c>
-      <c r="C39" t="n">
-        <v>647.509</v>
-      </c>
-      <c r="D39" t="n">
-        <v>561.14</v>
-      </c>
+      <c r="C39" t="inlineStr"/>
+      <c r="D39" t="inlineStr"/>
       <c r="E39" t="n">
         <v>469.217</v>
       </c>
@@ -2158,12 +1914,8 @@
       </c>
       <c r="G39" t="inlineStr"/>
       <c r="H39" t="inlineStr"/>
-      <c r="I39" t="n">
-        <v>560.0890000000001</v>
-      </c>
-      <c r="J39" t="n">
-        <v>794.652</v>
-      </c>
+      <c r="I39" t="inlineStr"/>
+      <c r="J39" t="inlineStr"/>
       <c r="K39" t="n">
         <v>648.9640000000001</v>
       </c>
@@ -2187,12 +1939,8 @@
       <c r="B40" t="n">
         <v>795.491</v>
       </c>
-      <c r="C40" t="n">
-        <v>648.131</v>
-      </c>
-      <c r="D40" t="n">
-        <v>552.9160000000001</v>
-      </c>
+      <c r="C40" t="inlineStr"/>
+      <c r="D40" t="inlineStr"/>
       <c r="E40" t="n">
         <v>468.857</v>
       </c>
@@ -2205,12 +1953,8 @@
       <c r="H40" t="n">
         <v>817.3869999999999</v>
       </c>
-      <c r="I40" t="n">
-        <v>553.598</v>
-      </c>
-      <c r="J40" t="n">
-        <v>789.088</v>
-      </c>
+      <c r="I40" t="inlineStr"/>
+      <c r="J40" t="inlineStr"/>
       <c r="K40" t="n">
         <v>648.4059999999999</v>
       </c>
@@ -2234,12 +1978,8 @@
       <c r="B41" t="n">
         <v>793.728</v>
       </c>
-      <c r="C41" t="n">
-        <v>648.5599999999999</v>
-      </c>
-      <c r="D41" t="n">
-        <v>544.909</v>
-      </c>
+      <c r="C41" t="inlineStr"/>
+      <c r="D41" t="inlineStr"/>
       <c r="E41" t="n">
         <v>467.376</v>
       </c>
@@ -2248,12 +1988,8 @@
       </c>
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr"/>
-      <c r="I41" t="n">
-        <v>546.356</v>
-      </c>
-      <c r="J41" t="n">
-        <v>779.544</v>
-      </c>
+      <c r="I41" t="inlineStr"/>
+      <c r="J41" t="inlineStr"/>
       <c r="K41" t="n">
         <v>648.35</v>
       </c>
@@ -2277,12 +2013,8 @@
       <c r="B42" t="n">
         <v>792.078</v>
       </c>
-      <c r="C42" t="n">
-        <v>649.725</v>
-      </c>
-      <c r="D42" t="n">
-        <v>539.566</v>
-      </c>
+      <c r="C42" t="inlineStr"/>
+      <c r="D42" t="inlineStr"/>
       <c r="E42" t="n">
         <v>466.475</v>
       </c>
@@ -2295,12 +2027,8 @@
       <c r="H42" t="n">
         <v>818.4160000000001</v>
       </c>
-      <c r="I42" t="n">
-        <v>537.533</v>
-      </c>
-      <c r="J42" t="n">
-        <v>771.082</v>
-      </c>
+      <c r="I42" t="inlineStr"/>
+      <c r="J42" t="inlineStr"/>
       <c r="K42" t="n">
         <v>648.0309999999999</v>
       </c>
@@ -2324,12 +2052,8 @@
       <c r="B43" t="n">
         <v>791.671</v>
       </c>
-      <c r="C43" t="n">
-        <v>649.28</v>
-      </c>
-      <c r="D43" t="n">
-        <v>533.061</v>
-      </c>
+      <c r="C43" t="inlineStr"/>
+      <c r="D43" t="inlineStr"/>
       <c r="E43" t="n">
         <v>464.449</v>
       </c>
@@ -2342,12 +2066,8 @@
       <c r="H43" t="n">
         <v>818.6079999999999</v>
       </c>
-      <c r="I43" t="n">
-        <v>533.919</v>
-      </c>
-      <c r="J43" t="n">
-        <v>763.2140000000001</v>
-      </c>
+      <c r="I43" t="inlineStr"/>
+      <c r="J43" t="inlineStr"/>
       <c r="K43" t="n">
         <v>648.53</v>
       </c>
@@ -2371,12 +2091,8 @@
       <c r="B44" t="n">
         <v>791.497</v>
       </c>
-      <c r="C44" t="n">
-        <v>650.092</v>
-      </c>
-      <c r="D44" t="n">
-        <v>529.514</v>
-      </c>
+      <c r="C44" t="inlineStr"/>
+      <c r="D44" t="inlineStr"/>
       <c r="E44" t="n">
         <v>464.311</v>
       </c>
@@ -2389,12 +2105,8 @@
       <c r="H44" t="n">
         <v>817.27</v>
       </c>
-      <c r="I44" t="n">
-        <v>528.346</v>
-      </c>
-      <c r="J44" t="n">
-        <v>754.273</v>
-      </c>
+      <c r="I44" t="inlineStr"/>
+      <c r="J44" t="inlineStr"/>
       <c r="K44" t="n">
         <v>649.3579999999999</v>
       </c>
@@ -2418,12 +2130,8 @@
       <c r="B45" t="n">
         <v>789.13</v>
       </c>
-      <c r="C45" t="n">
-        <v>649.165</v>
-      </c>
-      <c r="D45" t="n">
-        <v>524.716</v>
-      </c>
+      <c r="C45" t="inlineStr"/>
+      <c r="D45" t="inlineStr"/>
       <c r="E45" t="n">
         <v>463.179</v>
       </c>
@@ -2436,12 +2144,8 @@
       <c r="H45" t="n">
         <v>815.474</v>
       </c>
-      <c r="I45" t="n">
-        <v>524.222</v>
-      </c>
-      <c r="J45" t="n">
-        <v>743.72</v>
-      </c>
+      <c r="I45" t="inlineStr"/>
+      <c r="J45" t="inlineStr"/>
       <c r="K45" t="n">
         <v>649.663</v>
       </c>
@@ -2465,12 +2169,8 @@
       <c r="B46" t="n">
         <v>788.263</v>
       </c>
-      <c r="C46" t="n">
-        <v>646.877</v>
-      </c>
-      <c r="D46" t="n">
-        <v>521.226</v>
-      </c>
+      <c r="C46" t="inlineStr"/>
+      <c r="D46" t="inlineStr"/>
       <c r="E46" t="n">
         <v>461.91</v>
       </c>
@@ -2483,12 +2183,8 @@
       <c r="H46" t="n">
         <v>810.432</v>
       </c>
-      <c r="I46" t="n">
-        <v>520.689</v>
-      </c>
-      <c r="J46" t="n">
-        <v>733.317</v>
-      </c>
+      <c r="I46" t="inlineStr"/>
+      <c r="J46" t="inlineStr"/>
       <c r="K46" t="n">
         <v>649.476</v>
       </c>
@@ -2512,12 +2208,8 @@
       <c r="B47" t="n">
         <v>787.897</v>
       </c>
-      <c r="C47" t="n">
-        <v>646.088</v>
-      </c>
-      <c r="D47" t="n">
-        <v>518.191</v>
-      </c>
+      <c r="C47" t="inlineStr"/>
+      <c r="D47" t="inlineStr"/>
       <c r="E47" t="n">
         <v>462.46</v>
       </c>
@@ -2530,12 +2222,8 @@
       <c r="H47" t="n">
         <v>807.034</v>
       </c>
-      <c r="I47" t="n">
-        <v>515.578</v>
-      </c>
-      <c r="J47" t="n">
-        <v>721.443</v>
-      </c>
+      <c r="I47" t="inlineStr"/>
+      <c r="J47" t="inlineStr"/>
       <c r="K47" t="n">
         <v>649.357</v>
       </c>
@@ -2559,12 +2247,8 @@
       <c r="B48" t="n">
         <v>786.764</v>
       </c>
-      <c r="C48" t="n">
-        <v>645.119</v>
-      </c>
-      <c r="D48" t="n">
-        <v>515.8390000000001</v>
-      </c>
+      <c r="C48" t="inlineStr"/>
+      <c r="D48" t="inlineStr"/>
       <c r="E48" t="n">
         <v>461.544</v>
       </c>
@@ -2577,12 +2261,8 @@
       <c r="H48" t="n">
         <v>806.829</v>
       </c>
-      <c r="I48" t="n">
-        <v>513.865</v>
-      </c>
-      <c r="J48" t="n">
-        <v>713.559</v>
-      </c>
+      <c r="I48" t="inlineStr"/>
+      <c r="J48" t="inlineStr"/>
       <c r="K48" t="n">
         <v>648.223</v>
       </c>
@@ -2606,12 +2286,8 @@
       <c r="B49" t="n">
         <v>786.0839999999999</v>
       </c>
-      <c r="C49" t="n">
-        <v>643.804</v>
-      </c>
-      <c r="D49" t="n">
-        <v>513.182</v>
-      </c>
+      <c r="C49" t="inlineStr"/>
+      <c r="D49" t="inlineStr"/>
       <c r="E49" t="n">
         <v>462.485</v>
       </c>
@@ -2624,12 +2300,8 @@
       <c r="H49" t="n">
         <v>807.002</v>
       </c>
-      <c r="I49" t="n">
-        <v>507.812</v>
-      </c>
-      <c r="J49" t="n">
-        <v>704.12</v>
-      </c>
+      <c r="I49" t="inlineStr"/>
+      <c r="J49" t="inlineStr"/>
       <c r="K49" t="n">
         <v>648.154</v>
       </c>
@@ -2653,12 +2325,8 @@
       <c r="B50" t="n">
         <v>786.775</v>
       </c>
-      <c r="C50" t="n">
-        <v>643.653</v>
-      </c>
-      <c r="D50" t="n">
-        <v>509.628</v>
-      </c>
+      <c r="C50" t="inlineStr"/>
+      <c r="D50" t="inlineStr"/>
       <c r="E50" t="n">
         <v>462.357</v>
       </c>
@@ -2671,12 +2339,8 @@
       <c r="H50" t="n">
         <v>807.215</v>
       </c>
-      <c r="I50" t="n">
-        <v>504.494</v>
-      </c>
-      <c r="J50" t="n">
-        <v>695.172</v>
-      </c>
+      <c r="I50" t="inlineStr"/>
+      <c r="J50" t="inlineStr"/>
       <c r="K50" t="n">
         <v>647.208</v>
       </c>
@@ -2714,12 +2378,8 @@
       <c r="H51" t="n">
         <v>805.176</v>
       </c>
-      <c r="I51" t="n">
-        <v>500.985</v>
-      </c>
-      <c r="J51" t="n">
-        <v>686.974</v>
-      </c>
+      <c r="I51" t="inlineStr"/>
+      <c r="J51" t="inlineStr"/>
       <c r="K51" t="inlineStr"/>
       <c r="L51" t="inlineStr"/>
       <c r="M51" t="n">
@@ -2933,12 +2593,8 @@
       <c r="B58" t="n">
         <v>788.333</v>
       </c>
-      <c r="C58" t="n">
-        <v>649.05</v>
-      </c>
-      <c r="D58" t="n">
-        <v>770.578</v>
-      </c>
+      <c r="C58" t="inlineStr"/>
+      <c r="D58" t="inlineStr"/>
       <c r="E58" t="n">
         <v>471.324</v>
       </c>
@@ -2972,12 +2628,8 @@
       <c r="B59" t="n">
         <v>788.326</v>
       </c>
-      <c r="C59" t="n">
-        <v>649.938</v>
-      </c>
-      <c r="D59" t="n">
-        <v>765.736</v>
-      </c>
+      <c r="C59" t="inlineStr"/>
+      <c r="D59" t="inlineStr"/>
       <c r="E59" t="n">
         <v>472.686</v>
       </c>
@@ -2986,12 +2638,8 @@
       </c>
       <c r="G59" t="inlineStr"/>
       <c r="H59" t="inlineStr"/>
-      <c r="I59" t="n">
-        <v>476.055</v>
-      </c>
-      <c r="J59" t="n">
-        <v>621.126</v>
-      </c>
+      <c r="I59" t="inlineStr"/>
+      <c r="J59" t="inlineStr"/>
       <c r="K59" t="n">
         <v>640.391</v>
       </c>
@@ -3015,12 +2663,8 @@
       <c r="B60" t="n">
         <v>788.17</v>
       </c>
-      <c r="C60" t="n">
-        <v>649.409</v>
-      </c>
-      <c r="D60" t="n">
-        <v>761.51</v>
-      </c>
+      <c r="C60" t="inlineStr"/>
+      <c r="D60" t="inlineStr"/>
       <c r="E60" t="n">
         <v>473.543</v>
       </c>
@@ -3058,12 +2702,8 @@
       <c r="B61" t="n">
         <v>787.6319999999999</v>
       </c>
-      <c r="C61" t="n">
-        <v>649.372</v>
-      </c>
-      <c r="D61" t="n">
-        <v>756.011</v>
-      </c>
+      <c r="C61" t="inlineStr"/>
+      <c r="D61" t="inlineStr"/>
       <c r="E61" t="n">
         <v>476.588</v>
       </c>
@@ -3076,12 +2716,8 @@
       <c r="H61" t="n">
         <v>432.703</v>
       </c>
-      <c r="I61" t="n">
-        <v>473.079</v>
-      </c>
-      <c r="J61" t="n">
-        <v>603.148</v>
-      </c>
+      <c r="I61" t="inlineStr"/>
+      <c r="J61" t="inlineStr"/>
       <c r="K61" t="n">
         <v>643.463</v>
       </c>
@@ -3105,12 +2741,8 @@
       <c r="B62" t="n">
         <v>789.4160000000001</v>
       </c>
-      <c r="C62" t="n">
-        <v>648.134</v>
-      </c>
-      <c r="D62" t="n">
-        <v>751.956</v>
-      </c>
+      <c r="C62" t="inlineStr"/>
+      <c r="D62" t="inlineStr"/>
       <c r="E62" t="inlineStr"/>
       <c r="F62" t="inlineStr"/>
       <c r="G62" t="inlineStr"/>
@@ -3140,12 +2772,8 @@
       <c r="B63" t="n">
         <v>791.1369999999999</v>
       </c>
-      <c r="C63" t="n">
-        <v>647.979</v>
-      </c>
-      <c r="D63" t="n">
-        <v>750.667</v>
-      </c>
+      <c r="C63" t="inlineStr"/>
+      <c r="D63" t="inlineStr"/>
       <c r="E63" t="inlineStr"/>
       <c r="F63" t="inlineStr"/>
       <c r="G63" t="n">
@@ -3154,12 +2782,8 @@
       <c r="H63" t="n">
         <v>418.014</v>
       </c>
-      <c r="I63" t="n">
-        <v>479.591</v>
-      </c>
-      <c r="J63" t="n">
-        <v>473.207</v>
-      </c>
+      <c r="I63" t="inlineStr"/>
+      <c r="J63" t="inlineStr"/>
       <c r="K63" t="n">
         <v>647.496</v>
       </c>
@@ -3183,12 +2807,8 @@
       <c r="B64" t="n">
         <v>790.58</v>
       </c>
-      <c r="C64" t="n">
-        <v>648.045</v>
-      </c>
-      <c r="D64" t="n">
-        <v>750.823</v>
-      </c>
+      <c r="C64" t="inlineStr"/>
+      <c r="D64" t="inlineStr"/>
       <c r="E64" t="n">
         <v>470.594</v>
       </c>
@@ -3201,12 +2821,8 @@
       <c r="H64" t="n">
         <v>411.796</v>
       </c>
-      <c r="I64" t="n">
-        <v>484.162</v>
-      </c>
-      <c r="J64" t="n">
-        <v>463.708</v>
-      </c>
+      <c r="I64" t="inlineStr"/>
+      <c r="J64" t="inlineStr"/>
       <c r="K64" t="n">
         <v>648.811</v>
       </c>
@@ -3230,12 +2846,8 @@
       <c r="B65" t="n">
         <v>791.138</v>
       </c>
-      <c r="C65" t="n">
-        <v>648.268</v>
-      </c>
-      <c r="D65" t="n">
-        <v>750.2</v>
-      </c>
+      <c r="C65" t="inlineStr"/>
+      <c r="D65" t="inlineStr"/>
       <c r="E65" t="n">
         <v>469.35</v>
       </c>
@@ -3244,12 +2856,8 @@
       </c>
       <c r="G65" t="inlineStr"/>
       <c r="H65" t="inlineStr"/>
-      <c r="I65" t="n">
-        <v>485.174</v>
-      </c>
-      <c r="J65" t="n">
-        <v>454.536</v>
-      </c>
+      <c r="I65" t="inlineStr"/>
+      <c r="J65" t="inlineStr"/>
       <c r="K65" t="n">
         <v>650.0069999999999</v>
       </c>
@@ -3273,12 +2881,8 @@
       <c r="B66" t="n">
         <v>791.2</v>
       </c>
-      <c r="C66" t="n">
-        <v>650.0599999999999</v>
-      </c>
-      <c r="D66" t="n">
-        <v>743.439</v>
-      </c>
+      <c r="C66" t="inlineStr"/>
+      <c r="D66" t="inlineStr"/>
       <c r="E66" t="inlineStr"/>
       <c r="F66" t="inlineStr"/>
       <c r="G66" t="n">
@@ -3287,12 +2891,8 @@
       <c r="H66" t="n">
         <v>398.337</v>
       </c>
-      <c r="I66" t="n">
-        <v>488.169</v>
-      </c>
-      <c r="J66" t="n">
-        <v>447.323</v>
-      </c>
+      <c r="I66" t="inlineStr"/>
+      <c r="J66" t="inlineStr"/>
       <c r="K66" t="n">
         <v>649.8920000000001</v>
       </c>
@@ -3316,12 +2916,8 @@
       <c r="B67" t="n">
         <v>788.796</v>
       </c>
-      <c r="C67" t="n">
-        <v>648.097</v>
-      </c>
-      <c r="D67" t="n">
-        <v>736.081</v>
-      </c>
+      <c r="C67" t="inlineStr"/>
+      <c r="D67" t="inlineStr"/>
       <c r="E67" t="n">
         <v>468.369</v>
       </c>
@@ -3334,12 +2930,8 @@
       <c r="H67" t="n">
         <v>394.466</v>
       </c>
-      <c r="I67" t="n">
-        <v>489.495</v>
-      </c>
-      <c r="J67" t="n">
-        <v>438.859</v>
-      </c>
+      <c r="I67" t="inlineStr"/>
+      <c r="J67" t="inlineStr"/>
       <c r="K67" t="n">
         <v>649.99</v>
       </c>
@@ -3363,12 +2955,8 @@
       <c r="B68" t="n">
         <v>785.099</v>
       </c>
-      <c r="C68" t="n">
-        <v>647.244</v>
-      </c>
-      <c r="D68" t="n">
-        <v>724.59</v>
-      </c>
+      <c r="C68" t="inlineStr"/>
+      <c r="D68" t="inlineStr"/>
       <c r="E68" t="n">
         <v>468.132</v>
       </c>
@@ -3381,12 +2969,8 @@
       <c r="H68" t="n">
         <v>392.827</v>
       </c>
-      <c r="I68" t="n">
-        <v>490.756</v>
-      </c>
-      <c r="J68" t="n">
-        <v>432.797</v>
-      </c>
+      <c r="I68" t="inlineStr"/>
+      <c r="J68" t="inlineStr"/>
       <c r="K68" t="n">
         <v>650.732</v>
       </c>
@@ -3410,12 +2994,8 @@
       <c r="B69" t="n">
         <v>784.929</v>
       </c>
-      <c r="C69" t="n">
-        <v>647.244</v>
-      </c>
-      <c r="D69" t="n">
-        <v>724.59</v>
-      </c>
+      <c r="C69" t="inlineStr"/>
+      <c r="D69" t="inlineStr"/>
       <c r="E69" t="n">
         <v>468.132</v>
       </c>
@@ -3428,12 +3008,8 @@
       <c r="H69" t="n">
         <v>392.832</v>
       </c>
-      <c r="I69" t="n">
-        <v>490.743</v>
-      </c>
-      <c r="J69" t="n">
-        <v>432.852</v>
-      </c>
+      <c r="I69" t="inlineStr"/>
+      <c r="J69" t="inlineStr"/>
       <c r="K69" t="n">
         <v>650.713</v>
       </c>
@@ -3457,12 +3033,8 @@
       <c r="B70" t="n">
         <v>780.261</v>
       </c>
-      <c r="C70" t="n">
-        <v>646.671</v>
-      </c>
-      <c r="D70" t="n">
-        <v>715.206</v>
-      </c>
+      <c r="C70" t="inlineStr"/>
+      <c r="D70" t="inlineStr"/>
       <c r="E70" t="n">
         <v>466.725</v>
       </c>
@@ -3475,12 +3047,8 @@
       <c r="H70" t="n">
         <v>392.828</v>
       </c>
-      <c r="I70" t="n">
-        <v>493.989</v>
-      </c>
-      <c r="J70" t="n">
-        <v>426.084</v>
-      </c>
+      <c r="I70" t="inlineStr"/>
+      <c r="J70" t="inlineStr"/>
       <c r="K70" t="n">
         <v>649.683</v>
       </c>
@@ -3504,12 +3072,8 @@
       <c r="B71" t="n">
         <v>775.588</v>
       </c>
-      <c r="C71" t="n">
-        <v>643.691</v>
-      </c>
-      <c r="D71" t="n">
-        <v>717.213</v>
-      </c>
+      <c r="C71" t="inlineStr"/>
+      <c r="D71" t="inlineStr"/>
       <c r="E71" t="n">
         <v>465.305</v>
       </c>
@@ -3522,12 +3086,8 @@
       <c r="H71" t="n">
         <v>393.439</v>
       </c>
-      <c r="I71" t="n">
-        <v>501.824</v>
-      </c>
-      <c r="J71" t="n">
-        <v>410.021</v>
-      </c>
+      <c r="I71" t="inlineStr"/>
+      <c r="J71" t="inlineStr"/>
       <c r="K71" t="n">
         <v>650.053</v>
       </c>
@@ -3551,12 +3111,8 @@
       <c r="B72" t="n">
         <v>768.597</v>
       </c>
-      <c r="C72" t="n">
-        <v>643.609</v>
-      </c>
-      <c r="D72" t="n">
-        <v>718.097</v>
-      </c>
+      <c r="C72" t="inlineStr"/>
+      <c r="D72" t="inlineStr"/>
       <c r="E72" t="n">
         <v>464.886</v>
       </c>
@@ -3569,12 +3125,8 @@
       <c r="H72" t="n">
         <v>393.273</v>
       </c>
-      <c r="I72" t="n">
-        <v>507.127</v>
-      </c>
-      <c r="J72" t="n">
-        <v>403.403</v>
-      </c>
+      <c r="I72" t="inlineStr"/>
+      <c r="J72" t="inlineStr"/>
       <c r="K72" t="n">
         <v>649.583</v>
       </c>
@@ -3598,12 +3150,8 @@
       <c r="B73" t="n">
         <v>764.7670000000001</v>
       </c>
-      <c r="C73" t="n">
-        <v>641.7619999999999</v>
-      </c>
-      <c r="D73" t="n">
-        <v>715.4690000000001</v>
-      </c>
+      <c r="C73" t="inlineStr"/>
+      <c r="D73" t="inlineStr"/>
       <c r="E73" t="n">
         <v>464.977</v>
       </c>
@@ -3616,12 +3164,8 @@
       <c r="H73" t="n">
         <v>393.423</v>
       </c>
-      <c r="I73" t="n">
-        <v>508.718</v>
-      </c>
-      <c r="J73" t="n">
-        <v>400.846</v>
-      </c>
+      <c r="I73" t="inlineStr"/>
+      <c r="J73" t="inlineStr"/>
       <c r="K73" t="n">
         <v>649.5170000000001</v>
       </c>
@@ -3645,12 +3189,8 @@
       <c r="B74" t="n">
         <v>761.556</v>
       </c>
-      <c r="C74" t="n">
-        <v>640.138</v>
-      </c>
-      <c r="D74" t="n">
-        <v>713.254</v>
-      </c>
+      <c r="C74" t="inlineStr"/>
+      <c r="D74" t="inlineStr"/>
       <c r="E74" t="n">
         <v>465.068</v>
       </c>
@@ -3663,12 +3203,8 @@
       <c r="H74" t="n">
         <v>393.411</v>
       </c>
-      <c r="I74" t="n">
-        <v>510.796</v>
-      </c>
-      <c r="J74" t="n">
-        <v>396.805</v>
-      </c>
+      <c r="I74" t="inlineStr"/>
+      <c r="J74" t="inlineStr"/>
       <c r="K74" t="n">
         <v>649.417</v>
       </c>
@@ -3692,12 +3228,8 @@
       <c r="B75" t="n">
         <v>758.924</v>
       </c>
-      <c r="C75" t="n">
-        <v>638.443</v>
-      </c>
-      <c r="D75" t="n">
-        <v>709.774</v>
-      </c>
+      <c r="C75" t="inlineStr"/>
+      <c r="D75" t="inlineStr"/>
       <c r="E75" t="n">
         <v>464.642</v>
       </c>
@@ -3710,12 +3242,8 @@
       <c r="H75" t="n">
         <v>393.49</v>
       </c>
-      <c r="I75" t="n">
-        <v>518.3819999999999</v>
-      </c>
-      <c r="J75" t="n">
-        <v>390.103</v>
-      </c>
+      <c r="I75" t="inlineStr"/>
+      <c r="J75" t="inlineStr"/>
       <c r="K75" t="n">
         <v>649.999</v>
       </c>
@@ -3739,12 +3267,8 @@
       <c r="B76" t="n">
         <v>755.378</v>
       </c>
-      <c r="C76" t="n">
-        <v>634.819</v>
-      </c>
-      <c r="D76" t="n">
-        <v>704.146</v>
-      </c>
+      <c r="C76" t="inlineStr"/>
+      <c r="D76" t="inlineStr"/>
       <c r="E76" t="n">
         <v>464.209</v>
       </c>
@@ -3757,12 +3281,8 @@
       <c r="H76" t="n">
         <v>393.614</v>
       </c>
-      <c r="I76" t="n">
-        <v>522.265</v>
-      </c>
-      <c r="J76" t="n">
-        <v>383.422</v>
-      </c>
+      <c r="I76" t="inlineStr"/>
+      <c r="J76" t="inlineStr"/>
       <c r="K76" t="n">
         <v>650.039</v>
       </c>
@@ -3786,12 +3306,8 @@
       <c r="B77" t="n">
         <v>752.349</v>
       </c>
-      <c r="C77" t="n">
-        <v>631.795</v>
-      </c>
-      <c r="D77" t="n">
-        <v>699.279</v>
-      </c>
+      <c r="C77" t="inlineStr"/>
+      <c r="D77" t="inlineStr"/>
       <c r="E77" t="n">
         <v>463.684</v>
       </c>
@@ -3800,12 +3316,8 @@
       </c>
       <c r="G77" t="inlineStr"/>
       <c r="H77" t="inlineStr"/>
-      <c r="I77" t="n">
-        <v>528.41</v>
-      </c>
-      <c r="J77" t="n">
-        <v>377.057</v>
-      </c>
+      <c r="I77" t="inlineStr"/>
+      <c r="J77" t="inlineStr"/>
       <c r="K77" t="n">
         <v>650.178</v>
       </c>
@@ -3829,12 +3341,8 @@
       <c r="B78" t="n">
         <v>749.384</v>
       </c>
-      <c r="C78" t="n">
-        <v>627.348</v>
-      </c>
-      <c r="D78" t="n">
-        <v>694.127</v>
-      </c>
+      <c r="C78" t="inlineStr"/>
+      <c r="D78" t="inlineStr"/>
       <c r="E78" t="n">
         <v>463.346</v>
       </c>
@@ -3847,12 +3355,8 @@
       <c r="H78" t="n">
         <v>385.747</v>
       </c>
-      <c r="I78" t="n">
-        <v>534.927</v>
-      </c>
-      <c r="J78" t="n">
-        <v>369.476</v>
-      </c>
+      <c r="I78" t="inlineStr"/>
+      <c r="J78" t="inlineStr"/>
       <c r="K78" t="n">
         <v>650.354</v>
       </c>
@@ -3876,12 +3380,8 @@
       <c r="B79" t="n">
         <v>747.183</v>
       </c>
-      <c r="C79" t="n">
-        <v>622.8390000000001</v>
-      </c>
-      <c r="D79" t="n">
-        <v>689.457</v>
-      </c>
+      <c r="C79" t="inlineStr"/>
+      <c r="D79" t="inlineStr"/>
       <c r="E79" t="n">
         <v>463.005</v>
       </c>
@@ -3894,12 +3394,8 @@
       <c r="H79" t="n">
         <v>381.81</v>
       </c>
-      <c r="I79" t="n">
-        <v>538.255</v>
-      </c>
-      <c r="J79" t="n">
-        <v>363.496</v>
-      </c>
+      <c r="I79" t="inlineStr"/>
+      <c r="J79" t="inlineStr"/>
       <c r="K79" t="n">
         <v>650.99</v>
       </c>
@@ -3923,12 +3419,8 @@
       <c r="B80" t="n">
         <v>747.183</v>
       </c>
-      <c r="C80" t="n">
-        <v>622.872</v>
-      </c>
-      <c r="D80" t="n">
-        <v>689.52</v>
-      </c>
+      <c r="C80" t="inlineStr"/>
+      <c r="D80" t="inlineStr"/>
       <c r="E80" t="n">
         <v>463.005</v>
       </c>
@@ -3941,12 +3433,8 @@
       <c r="H80" t="n">
         <v>381.817</v>
       </c>
-      <c r="I80" t="n">
-        <v>538.218</v>
-      </c>
-      <c r="J80" t="n">
-        <v>363.564</v>
-      </c>
+      <c r="I80" t="inlineStr"/>
+      <c r="J80" t="inlineStr"/>
       <c r="K80" t="n">
         <v>650.99</v>
       </c>
@@ -3970,12 +3458,8 @@
       <c r="B81" t="n">
         <v>741.86</v>
       </c>
-      <c r="C81" t="n">
-        <v>621.823</v>
-      </c>
-      <c r="D81" t="n">
-        <v>689.09</v>
-      </c>
+      <c r="C81" t="inlineStr"/>
+      <c r="D81" t="inlineStr"/>
       <c r="E81" t="n">
         <v>462.467</v>
       </c>
@@ -3988,12 +3472,8 @@
       <c r="H81" t="n">
         <v>377.75</v>
       </c>
-      <c r="I81" t="n">
-        <v>542.955</v>
-      </c>
-      <c r="J81" t="n">
-        <v>359.611</v>
-      </c>
+      <c r="I81" t="inlineStr"/>
+      <c r="J81" t="inlineStr"/>
       <c r="K81" t="n">
         <v>651.082</v>
       </c>
@@ -4017,12 +3497,8 @@
       <c r="B82" t="n">
         <v>733.949</v>
       </c>
-      <c r="C82" t="n">
-        <v>621.535</v>
-      </c>
-      <c r="D82" t="n">
-        <v>688.53</v>
-      </c>
+      <c r="C82" t="inlineStr"/>
+      <c r="D82" t="inlineStr"/>
       <c r="E82" t="n">
         <v>463.525</v>
       </c>
@@ -4035,12 +3511,8 @@
       <c r="H82" t="n">
         <v>371.569</v>
       </c>
-      <c r="I82" t="n">
-        <v>544.407</v>
-      </c>
-      <c r="J82" t="n">
-        <v>358.662</v>
-      </c>
+      <c r="I82" t="inlineStr"/>
+      <c r="J82" t="inlineStr"/>
       <c r="K82" t="n">
         <v>651.241</v>
       </c>
@@ -4064,12 +3536,8 @@
       <c r="B83" t="n">
         <v>725.745</v>
       </c>
-      <c r="C83" t="n">
-        <v>620.321</v>
-      </c>
-      <c r="D83" t="n">
-        <v>681.944</v>
-      </c>
+      <c r="C83" t="inlineStr"/>
+      <c r="D83" t="inlineStr"/>
       <c r="E83" t="n">
         <v>464.18</v>
       </c>
@@ -4082,12 +3550,8 @@
       <c r="H83" t="n">
         <v>364.866</v>
       </c>
-      <c r="I83" t="n">
-        <v>544.116</v>
-      </c>
-      <c r="J83" t="n">
-        <v>359.017</v>
-      </c>
+      <c r="I83" t="inlineStr"/>
+      <c r="J83" t="inlineStr"/>
       <c r="K83" t="n">
         <v>649.861</v>
       </c>
@@ -4111,12 +3575,8 @@
       <c r="B84" t="n">
         <v>720.187</v>
       </c>
-      <c r="C84" t="n">
-        <v>618.987</v>
-      </c>
-      <c r="D84" t="n">
-        <v>674.76</v>
-      </c>
+      <c r="C84" t="inlineStr"/>
+      <c r="D84" t="inlineStr"/>
       <c r="E84" t="n">
         <v>463.694</v>
       </c>
@@ -4129,12 +3589,8 @@
       <c r="H84" t="n">
         <v>360.345</v>
       </c>
-      <c r="I84" t="n">
-        <v>544.093</v>
-      </c>
-      <c r="J84" t="n">
-        <v>359.242</v>
-      </c>
+      <c r="I84" t="inlineStr"/>
+      <c r="J84" t="inlineStr"/>
       <c r="K84" t="n">
         <v>649.981</v>
       </c>
@@ -4158,12 +3614,8 @@
       <c r="B85" t="n">
         <v>717.521</v>
       </c>
-      <c r="C85" t="n">
-        <v>619.8339999999999</v>
-      </c>
-      <c r="D85" t="n">
-        <v>670.103</v>
-      </c>
+      <c r="C85" t="inlineStr"/>
+      <c r="D85" t="inlineStr"/>
       <c r="E85" t="n">
         <v>464.748</v>
       </c>
@@ -4176,12 +3628,8 @@
       <c r="H85" t="n">
         <v>355.953</v>
       </c>
-      <c r="I85" t="n">
-        <v>543.996</v>
-      </c>
-      <c r="J85" t="n">
-        <v>359.141</v>
-      </c>
+      <c r="I85" t="inlineStr"/>
+      <c r="J85" t="inlineStr"/>
       <c r="K85" t="n">
         <v>650.14</v>
       </c>
@@ -4205,12 +3653,8 @@
       <c r="B86" t="n">
         <v>713.318</v>
       </c>
-      <c r="C86" t="n">
-        <v>619.436</v>
-      </c>
-      <c r="D86" t="n">
-        <v>664.976</v>
-      </c>
+      <c r="C86" t="inlineStr"/>
+      <c r="D86" t="inlineStr"/>
       <c r="E86" t="n">
         <v>464.272</v>
       </c>
@@ -4223,12 +3667,8 @@
       <c r="H86" t="n">
         <v>352.666</v>
       </c>
-      <c r="I86" t="n">
-        <v>543.944</v>
-      </c>
-      <c r="J86" t="n">
-        <v>359.363</v>
-      </c>
+      <c r="I86" t="inlineStr"/>
+      <c r="J86" t="inlineStr"/>
       <c r="K86" t="n">
         <v>648.165</v>
       </c>
@@ -4252,12 +3692,8 @@
       <c r="B87" t="n">
         <v>708.2190000000001</v>
       </c>
-      <c r="C87" t="n">
-        <v>618.881</v>
-      </c>
-      <c r="D87" t="n">
-        <v>656.602</v>
-      </c>
+      <c r="C87" t="inlineStr"/>
+      <c r="D87" t="inlineStr"/>
       <c r="E87" t="n">
         <v>464.128</v>
       </c>
@@ -4270,12 +3706,8 @@
       <c r="H87" t="n">
         <v>350.339</v>
       </c>
-      <c r="I87" t="n">
-        <v>543.929</v>
-      </c>
-      <c r="J87" t="n">
-        <v>359.69</v>
-      </c>
+      <c r="I87" t="inlineStr"/>
+      <c r="J87" t="inlineStr"/>
       <c r="K87" t="n">
         <v>646.802</v>
       </c>
@@ -4299,12 +3731,8 @@
       <c r="B88" t="n">
         <v>704.519</v>
       </c>
-      <c r="C88" t="n">
-        <v>620.878</v>
-      </c>
-      <c r="D88" t="n">
-        <v>648.937</v>
-      </c>
+      <c r="C88" t="inlineStr"/>
+      <c r="D88" t="inlineStr"/>
       <c r="E88" t="n">
         <v>465.156</v>
       </c>
@@ -4317,12 +3745,8 @@
       <c r="H88" t="n">
         <v>345.962</v>
       </c>
-      <c r="I88" t="n">
-        <v>543.9400000000001</v>
-      </c>
-      <c r="J88" t="n">
-        <v>359.434</v>
-      </c>
+      <c r="I88" t="inlineStr"/>
+      <c r="J88" t="inlineStr"/>
       <c r="K88" t="n">
         <v>641.568</v>
       </c>
@@ -4346,12 +3770,8 @@
       <c r="B89" t="n">
         <v>701.361</v>
       </c>
-      <c r="C89" t="n">
-        <v>620.539</v>
-      </c>
-      <c r="D89" t="n">
-        <v>642.3920000000001</v>
-      </c>
+      <c r="C89" t="inlineStr"/>
+      <c r="D89" t="inlineStr"/>
       <c r="E89" t="n">
         <v>464.347</v>
       </c>
@@ -4364,12 +3784,8 @@
       <c r="H89" t="n">
         <v>342.925</v>
       </c>
-      <c r="I89" t="n">
-        <v>543.967</v>
-      </c>
-      <c r="J89" t="n">
-        <v>359.29</v>
-      </c>
+      <c r="I89" t="inlineStr"/>
+      <c r="J89" t="inlineStr"/>
       <c r="K89" t="n">
         <v>639.356</v>
       </c>
@@ -4393,12 +3809,8 @@
       <c r="B90" t="n">
         <v>701.391</v>
       </c>
-      <c r="C90" t="n">
-        <v>620.539</v>
-      </c>
-      <c r="D90" t="n">
-        <v>642.3920000000001</v>
-      </c>
+      <c r="C90" t="inlineStr"/>
+      <c r="D90" t="inlineStr"/>
       <c r="E90" t="n">
         <v>464.352</v>
       </c>
@@ -4411,12 +3823,8 @@
       <c r="H90" t="n">
         <v>342.925</v>
       </c>
-      <c r="I90" t="n">
-        <v>544.021</v>
-      </c>
-      <c r="J90" t="n">
-        <v>359.134</v>
-      </c>
+      <c r="I90" t="inlineStr"/>
+      <c r="J90" t="inlineStr"/>
       <c r="K90" t="n">
         <v>639.356</v>
       </c>
@@ -4440,12 +3848,8 @@
       <c r="B91" t="n">
         <v>697.673</v>
       </c>
-      <c r="C91" t="n">
-        <v>620.865</v>
-      </c>
-      <c r="D91" t="n">
-        <v>636.752</v>
-      </c>
+      <c r="C91" t="inlineStr"/>
+      <c r="D91" t="inlineStr"/>
       <c r="E91" t="n">
         <v>464.161</v>
       </c>
@@ -4458,12 +3862,8 @@
       <c r="H91" t="n">
         <v>339.321</v>
       </c>
-      <c r="I91" t="n">
-        <v>543.985</v>
-      </c>
-      <c r="J91" t="n">
-        <v>359.456</v>
-      </c>
+      <c r="I91" t="inlineStr"/>
+      <c r="J91" t="inlineStr"/>
       <c r="K91" t="n">
         <v>635.597</v>
       </c>
@@ -4487,12 +3887,8 @@
       <c r="B92" t="n">
         <v>693.05</v>
       </c>
-      <c r="C92" t="n">
-        <v>622.813</v>
-      </c>
-      <c r="D92" t="n">
-        <v>634.628</v>
-      </c>
+      <c r="C92" t="inlineStr"/>
+      <c r="D92" t="inlineStr"/>
       <c r="E92" t="n">
         <v>465.959</v>
       </c>
@@ -4505,12 +3901,8 @@
       <c r="H92" t="n">
         <v>335.043</v>
       </c>
-      <c r="I92" t="n">
-        <v>543.9930000000001</v>
-      </c>
-      <c r="J92" t="n">
-        <v>359.34</v>
-      </c>
+      <c r="I92" t="inlineStr"/>
+      <c r="J92" t="inlineStr"/>
       <c r="K92" t="n">
         <v>630.485</v>
       </c>
@@ -4534,12 +3926,8 @@
       <c r="B93" t="n">
         <v>688.895</v>
       </c>
-      <c r="C93" t="n">
-        <v>626.063</v>
-      </c>
-      <c r="D93" t="n">
-        <v>632.2569999999999</v>
-      </c>
+      <c r="C93" t="inlineStr"/>
+      <c r="D93" t="inlineStr"/>
       <c r="E93" t="n">
         <v>466.114</v>
       </c>
@@ -4552,12 +3940,8 @@
       <c r="H93" t="n">
         <v>329.581</v>
       </c>
-      <c r="I93" t="n">
-        <v>544.0309999999999</v>
-      </c>
-      <c r="J93" t="n">
-        <v>359.353</v>
-      </c>
+      <c r="I93" t="inlineStr"/>
+      <c r="J93" t="inlineStr"/>
       <c r="K93" t="n">
         <v>624.144</v>
       </c>
@@ -4581,12 +3965,8 @@
       <c r="B94" t="n">
         <v>684.554</v>
       </c>
-      <c r="C94" t="n">
-        <v>625.807</v>
-      </c>
-      <c r="D94" t="n">
-        <v>630.045</v>
-      </c>
+      <c r="C94" t="inlineStr"/>
+      <c r="D94" t="inlineStr"/>
       <c r="E94" t="n">
         <v>467.25</v>
       </c>
@@ -4599,12 +3979,8 @@
       <c r="H94" t="n">
         <v>323.122</v>
       </c>
-      <c r="I94" t="n">
-        <v>544.147</v>
-      </c>
-      <c r="J94" t="n">
-        <v>359.366</v>
-      </c>
+      <c r="I94" t="inlineStr"/>
+      <c r="J94" t="inlineStr"/>
       <c r="K94" t="n">
         <v>618.349</v>
       </c>
@@ -4628,12 +4004,8 @@
       <c r="B95" t="n">
         <v>677.551</v>
       </c>
-      <c r="C95" t="n">
-        <v>626.769</v>
-      </c>
-      <c r="D95" t="n">
-        <v>623.702</v>
-      </c>
+      <c r="C95" t="inlineStr"/>
+      <c r="D95" t="inlineStr"/>
       <c r="E95" t="n">
         <v>469.645</v>
       </c>
@@ -4646,12 +4018,8 @@
       <c r="H95" t="n">
         <v>312.954</v>
       </c>
-      <c r="I95" t="n">
-        <v>550.383</v>
-      </c>
-      <c r="J95" t="n">
-        <v>343.681</v>
-      </c>
+      <c r="I95" t="inlineStr"/>
+      <c r="J95" t="inlineStr"/>
       <c r="K95" t="n">
         <v>604.727</v>
       </c>
@@ -4675,12 +4043,8 @@
       <c r="B96" t="n">
         <v>672.1950000000001</v>
       </c>
-      <c r="C96" t="n">
-        <v>626.717</v>
-      </c>
-      <c r="D96" t="n">
-        <v>619.9109999999999</v>
-      </c>
+      <c r="C96" t="inlineStr"/>
+      <c r="D96" t="inlineStr"/>
       <c r="E96" t="n">
         <v>469.993</v>
       </c>
@@ -4693,12 +4057,8 @@
       <c r="H96" t="n">
         <v>306.54</v>
       </c>
-      <c r="I96" t="n">
-        <v>555.33</v>
-      </c>
-      <c r="J96" t="n">
-        <v>337.651</v>
-      </c>
+      <c r="I96" t="inlineStr"/>
+      <c r="J96" t="inlineStr"/>
       <c r="K96" t="n">
         <v>598.9880000000001</v>
       </c>
@@ -4722,12 +4082,8 @@
       <c r="B97" t="n">
         <v>668.596</v>
       </c>
-      <c r="C97" t="n">
-        <v>627.9640000000001</v>
-      </c>
-      <c r="D97" t="n">
-        <v>612.682</v>
-      </c>
+      <c r="C97" t="inlineStr"/>
+      <c r="D97" t="inlineStr"/>
       <c r="E97" t="n">
         <v>471.654</v>
       </c>
@@ -4740,12 +4096,8 @@
       <c r="H97" t="n">
         <v>299.518</v>
       </c>
-      <c r="I97" t="n">
-        <v>558.715</v>
-      </c>
-      <c r="J97" t="n">
-        <v>330.682</v>
-      </c>
+      <c r="I97" t="inlineStr"/>
+      <c r="J97" t="inlineStr"/>
       <c r="K97" t="n">
         <v>592.39</v>
       </c>
@@ -4769,12 +4121,8 @@
       <c r="B98" t="n">
         <v>663.135</v>
       </c>
-      <c r="C98" t="n">
-        <v>630.496</v>
-      </c>
-      <c r="D98" t="n">
-        <v>603.876</v>
-      </c>
+      <c r="C98" t="inlineStr"/>
+      <c r="D98" t="inlineStr"/>
       <c r="E98" t="n">
         <v>471.615</v>
       </c>
@@ -4787,12 +4135,8 @@
       <c r="H98" t="n">
         <v>294.046</v>
       </c>
-      <c r="I98" t="n">
-        <v>560.4690000000001</v>
-      </c>
-      <c r="J98" t="n">
-        <v>325.505</v>
-      </c>
+      <c r="I98" t="inlineStr"/>
+      <c r="J98" t="inlineStr"/>
       <c r="K98" t="n">
         <v>587.842</v>
       </c>
@@ -4816,12 +4160,8 @@
       <c r="B99" t="n">
         <v>656.776</v>
       </c>
-      <c r="C99" t="n">
-        <v>630.211</v>
-      </c>
-      <c r="D99" t="n">
-        <v>595.821</v>
-      </c>
+      <c r="C99" t="inlineStr"/>
+      <c r="D99" t="inlineStr"/>
       <c r="E99" t="n">
         <v>472.429</v>
       </c>
@@ -4834,12 +4174,8 @@
       <c r="H99" t="n">
         <v>287.697</v>
       </c>
-      <c r="I99" t="n">
-        <v>563.5119999999999</v>
-      </c>
-      <c r="J99" t="n">
-        <v>320.521</v>
-      </c>
+      <c r="I99" t="inlineStr"/>
+      <c r="J99" t="inlineStr"/>
       <c r="K99" t="n">
         <v>581.144</v>
       </c>
@@ -4863,12 +4199,8 @@
       <c r="B100" t="n">
         <v>651.273</v>
       </c>
-      <c r="C100" t="n">
-        <v>630.652</v>
-      </c>
-      <c r="D100" t="n">
-        <v>587.91</v>
-      </c>
+      <c r="C100" t="inlineStr"/>
+      <c r="D100" t="inlineStr"/>
       <c r="E100" t="n">
         <v>475.299</v>
       </c>
@@ -4881,12 +4213,8 @@
       <c r="H100" t="n">
         <v>281.372</v>
       </c>
-      <c r="I100" t="n">
-        <v>567.91</v>
-      </c>
-      <c r="J100" t="n">
-        <v>314.535</v>
-      </c>
+      <c r="I100" t="inlineStr"/>
+      <c r="J100" t="inlineStr"/>
       <c r="K100" t="n">
         <v>578.311</v>
       </c>
@@ -4910,12 +4238,8 @@
       <c r="B101" t="n">
         <v>651.273</v>
       </c>
-      <c r="C101" t="n">
-        <v>630.6559999999999</v>
-      </c>
-      <c r="D101" t="n">
-        <v>588.054</v>
-      </c>
+      <c r="C101" t="inlineStr"/>
+      <c r="D101" t="inlineStr"/>
       <c r="E101" t="n">
         <v>475.299</v>
       </c>
@@ -4928,12 +4252,8 @@
       <c r="H101" t="n">
         <v>281.557</v>
       </c>
-      <c r="I101" t="n">
-        <v>567.7430000000001</v>
-      </c>
-      <c r="J101" t="n">
-        <v>314.805</v>
-      </c>
+      <c r="I101" t="inlineStr"/>
+      <c r="J101" t="inlineStr"/>
       <c r="K101" t="n">
         <v>578.3150000000001</v>
       </c>
@@ -4957,12 +4277,8 @@
       <c r="B102" t="n">
         <v>648.7859999999999</v>
       </c>
-      <c r="C102" t="n">
-        <v>631.302</v>
-      </c>
-      <c r="D102" t="n">
-        <v>579.538</v>
-      </c>
+      <c r="C102" t="inlineStr"/>
+      <c r="D102" t="inlineStr"/>
       <c r="E102" t="n">
         <v>475.356</v>
       </c>
@@ -4975,12 +4291,8 @@
       <c r="H102" t="n">
         <v>277.52</v>
       </c>
-      <c r="I102" t="n">
-        <v>572.328</v>
-      </c>
-      <c r="J102" t="n">
-        <v>306.567</v>
-      </c>
+      <c r="I102" t="inlineStr"/>
+      <c r="J102" t="inlineStr"/>
       <c r="K102" t="n">
         <v>571.681</v>
       </c>
@@ -5004,12 +4316,8 @@
       <c r="B103" t="n">
         <v>643.187</v>
       </c>
-      <c r="C103" t="n">
-        <v>631.343</v>
-      </c>
-      <c r="D103" t="n">
-        <v>571.657</v>
-      </c>
+      <c r="C103" t="inlineStr"/>
+      <c r="D103" t="inlineStr"/>
       <c r="E103" t="n">
         <v>476.811</v>
       </c>
@@ -5022,12 +4330,8 @@
       <c r="H103" t="n">
         <v>272.627</v>
       </c>
-      <c r="I103" t="n">
-        <v>576.2859999999999</v>
-      </c>
-      <c r="J103" t="n">
-        <v>301.021</v>
-      </c>
+      <c r="I103" t="inlineStr"/>
+      <c r="J103" t="inlineStr"/>
       <c r="K103" t="n">
         <v>565.487</v>
       </c>
@@ -5051,12 +4355,8 @@
       <c r="B104" t="n">
         <v>637.917</v>
       </c>
-      <c r="C104" t="n">
-        <v>631.585</v>
-      </c>
-      <c r="D104" t="n">
-        <v>564.849</v>
-      </c>
+      <c r="C104" t="inlineStr"/>
+      <c r="D104" t="inlineStr"/>
       <c r="E104" t="n">
         <v>479.713</v>
       </c>
@@ -5069,12 +4369,8 @@
       <c r="H104" t="n">
         <v>268.376</v>
       </c>
-      <c r="I104" t="n">
-        <v>578.9640000000001</v>
-      </c>
-      <c r="J104" t="n">
-        <v>294.989</v>
-      </c>
+      <c r="I104" t="inlineStr"/>
+      <c r="J104" t="inlineStr"/>
       <c r="K104" t="n">
         <v>555.712</v>
       </c>
@@ -5098,12 +4394,8 @@
       <c r="B105" t="n">
         <v>633.895</v>
       </c>
-      <c r="C105" t="n">
-        <v>631.707</v>
-      </c>
-      <c r="D105" t="n">
-        <v>555.873</v>
-      </c>
+      <c r="C105" t="inlineStr"/>
+      <c r="D105" t="inlineStr"/>
       <c r="E105" t="n">
         <v>481.126</v>
       </c>
@@ -5116,12 +4408,8 @@
       <c r="H105" t="n">
         <v>265.602</v>
       </c>
-      <c r="I105" t="n">
-        <v>580.1130000000001</v>
-      </c>
-      <c r="J105" t="n">
-        <v>291.944</v>
-      </c>
+      <c r="I105" t="inlineStr"/>
+      <c r="J105" t="inlineStr"/>
       <c r="K105" t="n">
         <v>549.515</v>
       </c>
@@ -5145,12 +4433,8 @@
       <c r="B106" t="n">
         <v>628.725</v>
       </c>
-      <c r="C106" t="n">
-        <v>631.349</v>
-      </c>
-      <c r="D106" t="n">
-        <v>545.644</v>
-      </c>
+      <c r="C106" t="inlineStr"/>
+      <c r="D106" t="inlineStr"/>
       <c r="E106" t="n">
         <v>482.147</v>
       </c>
@@ -5163,12 +4447,8 @@
       <c r="H106" t="n">
         <v>261.493</v>
       </c>
-      <c r="I106" t="n">
-        <v>582.12</v>
-      </c>
-      <c r="J106" t="n">
-        <v>287.765</v>
-      </c>
+      <c r="I106" t="inlineStr"/>
+      <c r="J106" t="inlineStr"/>
       <c r="K106" t="n">
         <v>541.7809999999999</v>
       </c>
@@ -5192,12 +4472,8 @@
       <c r="B107" t="n">
         <v>618.141</v>
       </c>
-      <c r="C107" t="n">
-        <v>629.968</v>
-      </c>
-      <c r="D107" t="n">
-        <v>527.601</v>
-      </c>
+      <c r="C107" t="inlineStr"/>
+      <c r="D107" t="inlineStr"/>
       <c r="E107" t="n">
         <v>487.739</v>
       </c>
@@ -5210,12 +4486,8 @@
       <c r="H107" t="n">
         <v>254.038</v>
       </c>
-      <c r="I107" t="n">
-        <v>586.751</v>
-      </c>
-      <c r="J107" t="n">
-        <v>277.978</v>
-      </c>
+      <c r="I107" t="inlineStr"/>
+      <c r="J107" t="inlineStr"/>
       <c r="K107" t="n">
         <v>527.367</v>
       </c>
@@ -5239,12 +4511,8 @@
       <c r="B108" t="n">
         <v>613.998</v>
       </c>
-      <c r="C108" t="n">
-        <v>629.9930000000001</v>
-      </c>
-      <c r="D108" t="n">
-        <v>519.2619999999999</v>
-      </c>
+      <c r="C108" t="inlineStr"/>
+      <c r="D108" t="inlineStr"/>
       <c r="E108" t="n">
         <v>489.161</v>
       </c>
@@ -5257,12 +4525,8 @@
       <c r="H108" t="n">
         <v>249.204</v>
       </c>
-      <c r="I108" t="n">
-        <v>589.4829999999999</v>
-      </c>
-      <c r="J108" t="n">
-        <v>271.297</v>
-      </c>
+      <c r="I108" t="inlineStr"/>
+      <c r="J108" t="inlineStr"/>
       <c r="K108" t="n">
         <v>518.737</v>
       </c>
@@ -5286,12 +4550,8 @@
       <c r="B109" t="n">
         <v>608.48</v>
       </c>
-      <c r="C109" t="n">
-        <v>629.852</v>
-      </c>
-      <c r="D109" t="n">
-        <v>510.758</v>
-      </c>
+      <c r="C109" t="inlineStr"/>
+      <c r="D109" t="inlineStr"/>
       <c r="E109" t="n">
         <v>493.428</v>
       </c>
@@ -5304,12 +4564,8 @@
       <c r="H109" t="n">
         <v>246.018</v>
       </c>
-      <c r="I109" t="n">
-        <v>592.275</v>
-      </c>
-      <c r="J109" t="n">
-        <v>265.629</v>
-      </c>
+      <c r="I109" t="inlineStr"/>
+      <c r="J109" t="inlineStr"/>
       <c r="K109" t="n">
         <v>512.083</v>
       </c>
@@ -5333,12 +4589,8 @@
       <c r="B110" t="n">
         <v>604.3</v>
       </c>
-      <c r="C110" t="n">
-        <v>629.038</v>
-      </c>
-      <c r="D110" t="n">
-        <v>501.691</v>
-      </c>
+      <c r="C110" t="inlineStr"/>
+      <c r="D110" t="inlineStr"/>
       <c r="E110" t="n">
         <v>494.223</v>
       </c>
@@ -5351,12 +4603,8 @@
       <c r="H110" t="n">
         <v>243.95</v>
       </c>
-      <c r="I110" t="n">
-        <v>593.681</v>
-      </c>
-      <c r="J110" t="n">
-        <v>260.653</v>
-      </c>
+      <c r="I110" t="inlineStr"/>
+      <c r="J110" t="inlineStr"/>
       <c r="K110" t="inlineStr"/>
       <c r="L110" t="inlineStr"/>
       <c r="M110" t="inlineStr"/>
@@ -5372,12 +4620,8 @@
       <c r="B111" t="n">
         <v>604.3</v>
       </c>
-      <c r="C111" t="n">
-        <v>629.022</v>
-      </c>
-      <c r="D111" t="n">
-        <v>501.586</v>
-      </c>
+      <c r="C111" t="inlineStr"/>
+      <c r="D111" t="inlineStr"/>
       <c r="E111" t="n">
         <v>494.222</v>
       </c>
@@ -5390,12 +4634,8 @@
       <c r="H111" t="n">
         <v>243.971</v>
       </c>
-      <c r="I111" t="n">
-        <v>593.6559999999999</v>
-      </c>
-      <c r="J111" t="n">
-        <v>260.752</v>
-      </c>
+      <c r="I111" t="inlineStr"/>
+      <c r="J111" t="inlineStr"/>
       <c r="K111" t="inlineStr"/>
       <c r="L111" t="inlineStr"/>
       <c r="M111" t="inlineStr"/>
@@ -5411,12 +4651,8 @@
       <c r="B112" t="n">
         <v>599.545</v>
       </c>
-      <c r="C112" t="n">
-        <v>629.268</v>
-      </c>
-      <c r="D112" t="n">
-        <v>492.798</v>
-      </c>
+      <c r="C112" t="inlineStr"/>
+      <c r="D112" t="inlineStr"/>
       <c r="E112" t="n">
         <v>492.42</v>
       </c>
@@ -5429,12 +4665,8 @@
       <c r="H112" t="n">
         <v>239.958</v>
       </c>
-      <c r="I112" t="n">
-        <v>595.924</v>
-      </c>
-      <c r="J112" t="n">
-        <v>255.065</v>
-      </c>
+      <c r="I112" t="inlineStr"/>
+      <c r="J112" t="inlineStr"/>
       <c r="K112" t="inlineStr"/>
       <c r="L112" t="inlineStr"/>
       <c r="M112" t="inlineStr"/>
@@ -5450,12 +4682,8 @@
       <c r="B113" t="n">
         <v>594.369</v>
       </c>
-      <c r="C113" t="n">
-        <v>629.476</v>
-      </c>
-      <c r="D113" t="n">
-        <v>484.579</v>
-      </c>
+      <c r="C113" t="inlineStr"/>
+      <c r="D113" t="inlineStr"/>
       <c r="E113" t="n">
         <v>491.775</v>
       </c>
@@ -5468,12 +4696,8 @@
       <c r="H113" t="n">
         <v>236.047</v>
       </c>
-      <c r="I113" t="n">
-        <v>600.436</v>
-      </c>
-      <c r="J113" t="n">
-        <v>247.634</v>
-      </c>
+      <c r="I113" t="inlineStr"/>
+      <c r="J113" t="inlineStr"/>
       <c r="K113" t="inlineStr"/>
       <c r="L113" t="inlineStr"/>
       <c r="M113" t="inlineStr"/>
@@ -5489,12 +4713,8 @@
       <c r="B114" t="n">
         <v>591.496</v>
       </c>
-      <c r="C114" t="n">
-        <v>628.789</v>
-      </c>
-      <c r="D114" t="n">
-        <v>473.28</v>
-      </c>
+      <c r="C114" t="inlineStr"/>
+      <c r="D114" t="inlineStr"/>
       <c r="E114" t="n">
         <v>491.361</v>
       </c>
@@ -5507,12 +4727,8 @@
       <c r="H114" t="n">
         <v>233.944</v>
       </c>
-      <c r="I114" t="n">
-        <v>602.924</v>
-      </c>
-      <c r="J114" t="n">
-        <v>242.413</v>
-      </c>
+      <c r="I114" t="inlineStr"/>
+      <c r="J114" t="inlineStr"/>
       <c r="K114" t="inlineStr"/>
       <c r="L114" t="inlineStr"/>
       <c r="M114" t="inlineStr"/>
@@ -5528,12 +4744,8 @@
       <c r="B115" t="n">
         <v>588.754</v>
       </c>
-      <c r="C115" t="n">
-        <v>628.924</v>
-      </c>
-      <c r="D115" t="n">
-        <v>464.18</v>
-      </c>
+      <c r="C115" t="inlineStr"/>
+      <c r="D115" t="inlineStr"/>
       <c r="E115" t="n">
         <v>491.707</v>
       </c>
@@ -5546,12 +4758,8 @@
       <c r="H115" t="n">
         <v>233.596</v>
       </c>
-      <c r="I115" t="n">
-        <v>606.545</v>
-      </c>
-      <c r="J115" t="n">
-        <v>237.133</v>
-      </c>
+      <c r="I115" t="inlineStr"/>
+      <c r="J115" t="inlineStr"/>
       <c r="K115" t="inlineStr"/>
       <c r="L115" t="inlineStr"/>
       <c r="M115" t="inlineStr"/>
@@ -5567,12 +4775,8 @@
       <c r="B116" t="n">
         <v>582.723</v>
       </c>
-      <c r="C116" t="n">
-        <v>629.425</v>
-      </c>
-      <c r="D116" t="n">
-        <v>461.562</v>
-      </c>
+      <c r="C116" t="inlineStr"/>
+      <c r="D116" t="inlineStr"/>
       <c r="E116" t="n">
         <v>491.254</v>
       </c>
@@ -5581,12 +4785,8 @@
       </c>
       <c r="G116" t="inlineStr"/>
       <c r="H116" t="inlineStr"/>
-      <c r="I116" t="n">
-        <v>513.35</v>
-      </c>
-      <c r="J116" t="n">
-        <v>236.875</v>
-      </c>
+      <c r="I116" t="inlineStr"/>
+      <c r="J116" t="inlineStr"/>
       <c r="K116" t="inlineStr"/>
       <c r="L116" t="inlineStr"/>
       <c r="M116" t="n">
@@ -5606,12 +4806,8 @@
       <c r="B117" t="n">
         <v>577.634</v>
       </c>
-      <c r="C117" t="n">
-        <v>629.359</v>
-      </c>
-      <c r="D117" t="n">
-        <v>462.175</v>
-      </c>
+      <c r="C117" t="inlineStr"/>
+      <c r="D117" t="inlineStr"/>
       <c r="E117" t="n">
         <v>491.293</v>
       </c>
@@ -5620,12 +4816,8 @@
       </c>
       <c r="G117" t="inlineStr"/>
       <c r="H117" t="inlineStr"/>
-      <c r="I117" t="n">
-        <v>517.963</v>
-      </c>
-      <c r="J117" t="n">
-        <v>236.785</v>
-      </c>
+      <c r="I117" t="inlineStr"/>
+      <c r="J117" t="inlineStr"/>
       <c r="K117" t="inlineStr"/>
       <c r="L117" t="inlineStr"/>
       <c r="M117" t="n">
@@ -5645,12 +4837,8 @@
       <c r="B118" t="n">
         <v>574.0359999999999</v>
       </c>
-      <c r="C118" t="n">
-        <v>629.3339999999999</v>
-      </c>
-      <c r="D118" t="n">
-        <v>461.969</v>
-      </c>
+      <c r="C118" t="inlineStr"/>
+      <c r="D118" t="inlineStr"/>
       <c r="E118" t="n">
         <v>491.519</v>
       </c>
@@ -5659,12 +4847,8 @@
       </c>
       <c r="G118" t="inlineStr"/>
       <c r="H118" t="inlineStr"/>
-      <c r="I118" t="n">
-        <v>526.41</v>
-      </c>
-      <c r="J118" t="n">
-        <v>235.58</v>
-      </c>
+      <c r="I118" t="inlineStr"/>
+      <c r="J118" t="inlineStr"/>
       <c r="K118" t="inlineStr"/>
       <c r="L118" t="inlineStr"/>
       <c r="M118" t="n">
@@ -5684,12 +4868,8 @@
       <c r="B119" t="n">
         <v>562.593</v>
       </c>
-      <c r="C119" t="n">
-        <v>631.7859999999999</v>
-      </c>
-      <c r="D119" t="n">
-        <v>449.93</v>
-      </c>
+      <c r="C119" t="inlineStr"/>
+      <c r="D119" t="inlineStr"/>
       <c r="E119" t="n">
         <v>491.426</v>
       </c>
@@ -5698,12 +4878,8 @@
       </c>
       <c r="G119" t="inlineStr"/>
       <c r="H119" t="inlineStr"/>
-      <c r="I119" t="n">
-        <v>543.6</v>
-      </c>
-      <c r="J119" t="n">
-        <v>232.535</v>
-      </c>
+      <c r="I119" t="inlineStr"/>
+      <c r="J119" t="inlineStr"/>
       <c r="K119" t="inlineStr"/>
       <c r="L119" t="inlineStr"/>
       <c r="M119" t="n">
@@ -5723,12 +4899,8 @@
       <c r="B120" t="n">
         <v>557.783</v>
       </c>
-      <c r="C120" t="n">
-        <v>632.617</v>
-      </c>
-      <c r="D120" t="n">
-        <v>443.726</v>
-      </c>
+      <c r="C120" t="inlineStr"/>
+      <c r="D120" t="inlineStr"/>
       <c r="E120" t="n">
         <v>491.77</v>
       </c>
@@ -5737,12 +4909,8 @@
       </c>
       <c r="G120" t="inlineStr"/>
       <c r="H120" t="inlineStr"/>
-      <c r="I120" t="n">
-        <v>550.9829999999999</v>
-      </c>
-      <c r="J120" t="n">
-        <v>230.447</v>
-      </c>
+      <c r="I120" t="inlineStr"/>
+      <c r="J120" t="inlineStr"/>
       <c r="K120" t="inlineStr"/>
       <c r="L120" t="inlineStr"/>
       <c r="M120" t="n">
@@ -5762,12 +4930,8 @@
       <c r="B121" t="n">
         <v>554.766</v>
       </c>
-      <c r="C121" t="n">
-        <v>635.3150000000001</v>
-      </c>
-      <c r="D121" t="n">
-        <v>435.394</v>
-      </c>
+      <c r="C121" t="inlineStr"/>
+      <c r="D121" t="inlineStr"/>
       <c r="E121" t="n">
         <v>493.448</v>
       </c>
@@ -5776,12 +4940,8 @@
       </c>
       <c r="G121" t="inlineStr"/>
       <c r="H121" t="inlineStr"/>
-      <c r="I121" t="n">
-        <v>560.491</v>
-      </c>
-      <c r="J121" t="n">
-        <v>229.594</v>
-      </c>
+      <c r="I121" t="inlineStr"/>
+      <c r="J121" t="inlineStr"/>
       <c r="K121" t="inlineStr"/>
       <c r="L121" t="inlineStr"/>
       <c r="M121" t="n">
@@ -5801,12 +4961,8 @@
       <c r="B122" t="n">
         <v>554.4829999999999</v>
       </c>
-      <c r="C122" t="n">
-        <v>635.404</v>
-      </c>
-      <c r="D122" t="n">
-        <v>435.246</v>
-      </c>
+      <c r="C122" t="inlineStr"/>
+      <c r="D122" t="inlineStr"/>
       <c r="E122" t="n">
         <v>493.494</v>
       </c>
@@ -5815,12 +4971,8 @@
       </c>
       <c r="G122" t="inlineStr"/>
       <c r="H122" t="inlineStr"/>
-      <c r="I122" t="n">
-        <v>560.336</v>
-      </c>
-      <c r="J122" t="n">
-        <v>229.65</v>
-      </c>
+      <c r="I122" t="inlineStr"/>
+      <c r="J122" t="inlineStr"/>
       <c r="K122" t="inlineStr"/>
       <c r="L122" t="inlineStr"/>
       <c r="M122" t="n">
@@ -5840,12 +4992,8 @@
       <c r="B123" t="n">
         <v>550.703</v>
       </c>
-      <c r="C123" t="n">
-        <v>638.159</v>
-      </c>
-      <c r="D123" t="n">
-        <v>427.456</v>
-      </c>
+      <c r="C123" t="inlineStr"/>
+      <c r="D123" t="inlineStr"/>
       <c r="E123" t="n">
         <v>495.169</v>
       </c>
@@ -5854,12 +5002,8 @@
       </c>
       <c r="G123" t="inlineStr"/>
       <c r="H123" t="inlineStr"/>
-      <c r="I123" t="n">
-        <v>567.735</v>
-      </c>
-      <c r="J123" t="n">
-        <v>225.144</v>
-      </c>
+      <c r="I123" t="inlineStr"/>
+      <c r="J123" t="inlineStr"/>
       <c r="K123" t="inlineStr"/>
       <c r="L123" t="inlineStr"/>
       <c r="M123" t="n">
@@ -5879,12 +5023,8 @@
       <c r="B124" t="n">
         <v>545.367</v>
       </c>
-      <c r="C124" t="n">
-        <v>639.5119999999999</v>
-      </c>
-      <c r="D124" t="n">
-        <v>419.574</v>
-      </c>
+      <c r="C124" t="inlineStr"/>
+      <c r="D124" t="inlineStr"/>
       <c r="E124" t="n">
         <v>495.083</v>
       </c>
@@ -5893,12 +5033,8 @@
       </c>
       <c r="G124" t="inlineStr"/>
       <c r="H124" t="inlineStr"/>
-      <c r="I124" t="n">
-        <v>573.771</v>
-      </c>
-      <c r="J124" t="n">
-        <v>220.359</v>
-      </c>
+      <c r="I124" t="inlineStr"/>
+      <c r="J124" t="inlineStr"/>
       <c r="K124" t="inlineStr"/>
       <c r="L124" t="inlineStr"/>
       <c r="M124" t="n">
@@ -5918,12 +5054,8 @@
       <c r="B125" t="n">
         <v>540.5119999999999</v>
       </c>
-      <c r="C125" t="n">
-        <v>639.516</v>
-      </c>
-      <c r="D125" t="n">
-        <v>417.664</v>
-      </c>
+      <c r="C125" t="inlineStr"/>
+      <c r="D125" t="inlineStr"/>
       <c r="E125" t="n">
         <v>496.105</v>
       </c>
@@ -5932,12 +5064,8 @@
       </c>
       <c r="G125" t="inlineStr"/>
       <c r="H125" t="inlineStr"/>
-      <c r="I125" t="n">
-        <v>577.61</v>
-      </c>
-      <c r="J125" t="n">
-        <v>217.626</v>
-      </c>
+      <c r="I125" t="inlineStr"/>
+      <c r="J125" t="inlineStr"/>
       <c r="K125" t="inlineStr"/>
       <c r="L125" t="inlineStr"/>
       <c r="M125" t="n">
@@ -5957,12 +5085,8 @@
       <c r="B126" t="n">
         <v>536.564</v>
       </c>
-      <c r="C126" t="n">
-        <v>639.561</v>
-      </c>
-      <c r="D126" t="n">
-        <v>417.271</v>
-      </c>
+      <c r="C126" t="inlineStr"/>
+      <c r="D126" t="inlineStr"/>
       <c r="E126" t="n">
         <v>497.639</v>
       </c>
@@ -5971,12 +5095,8 @@
       </c>
       <c r="G126" t="inlineStr"/>
       <c r="H126" t="inlineStr"/>
-      <c r="I126" t="n">
-        <v>578.574</v>
-      </c>
-      <c r="J126" t="n">
-        <v>222.946</v>
-      </c>
+      <c r="I126" t="inlineStr"/>
+      <c r="J126" t="inlineStr"/>
       <c r="K126" t="inlineStr"/>
       <c r="L126" t="inlineStr"/>
       <c r="M126" t="n">
@@ -5996,12 +5116,8 @@
       <c r="B127" t="n">
         <v>531.841</v>
       </c>
-      <c r="C127" t="n">
-        <v>639.6130000000001</v>
-      </c>
-      <c r="D127" t="n">
-        <v>417.389</v>
-      </c>
+      <c r="C127" t="inlineStr"/>
+      <c r="D127" t="inlineStr"/>
       <c r="E127" t="n">
         <v>498.853</v>
       </c>
@@ -6010,12 +5126,8 @@
       </c>
       <c r="G127" t="inlineStr"/>
       <c r="H127" t="inlineStr"/>
-      <c r="I127" t="n">
-        <v>580.574</v>
-      </c>
-      <c r="J127" t="n">
-        <v>224.429</v>
-      </c>
+      <c r="I127" t="inlineStr"/>
+      <c r="J127" t="inlineStr"/>
       <c r="K127" t="inlineStr"/>
       <c r="L127" t="inlineStr"/>
       <c r="M127" t="n">
@@ -6035,12 +5147,8 @@
       <c r="B128" t="n">
         <v>523.903</v>
       </c>
-      <c r="C128" t="n">
-        <v>639.477</v>
-      </c>
-      <c r="D128" t="n">
-        <v>417.769</v>
-      </c>
+      <c r="C128" t="inlineStr"/>
+      <c r="D128" t="inlineStr"/>
       <c r="E128" t="n">
         <v>501.975</v>
       </c>
@@ -6070,12 +5178,8 @@
       <c r="B129" t="n">
         <v>519.475</v>
       </c>
-      <c r="C129" t="n">
-        <v>639.629</v>
-      </c>
-      <c r="D129" t="n">
-        <v>417.457</v>
-      </c>
+      <c r="C129" t="inlineStr"/>
+      <c r="D129" t="inlineStr"/>
       <c r="E129" t="n">
         <v>501.967</v>
       </c>
@@ -6105,12 +5209,8 @@
       <c r="B130" t="n">
         <v>516.595</v>
       </c>
-      <c r="C130" t="n">
-        <v>639.557</v>
-      </c>
-      <c r="D130" t="n">
-        <v>416.417</v>
-      </c>
+      <c r="C130" t="inlineStr"/>
+      <c r="D130" t="inlineStr"/>
       <c r="E130" t="n">
         <v>506.265</v>
       </c>
@@ -6140,12 +5240,8 @@
       <c r="B131" t="n">
         <v>506.161</v>
       </c>
-      <c r="C131" t="n">
-        <v>640.754</v>
-      </c>
-      <c r="D131" t="n">
-        <v>410.79</v>
-      </c>
+      <c r="C131" t="inlineStr"/>
+      <c r="D131" t="inlineStr"/>
       <c r="E131" t="n">
         <v>513.649</v>
       </c>
@@ -6175,12 +5271,8 @@
       <c r="B132" t="n">
         <v>503.232</v>
       </c>
-      <c r="C132" t="n">
-        <v>640.602</v>
-      </c>
-      <c r="D132" t="n">
-        <v>410.527</v>
-      </c>
+      <c r="C132" t="inlineStr"/>
+      <c r="D132" t="inlineStr"/>
       <c r="E132" t="n">
         <v>517.0410000000001</v>
       </c>
@@ -6210,12 +5302,8 @@
       <c r="B133" t="n">
         <v>503.184</v>
       </c>
-      <c r="C133" t="n">
-        <v>640.6180000000001</v>
-      </c>
-      <c r="D133" t="n">
-        <v>410.437</v>
-      </c>
+      <c r="C133" t="inlineStr"/>
+      <c r="D133" t="inlineStr"/>
       <c r="E133" t="n">
         <v>517.121</v>
       </c>
@@ -6245,12 +5333,8 @@
       <c r="B134" t="n">
         <v>500.118</v>
       </c>
-      <c r="C134" t="n">
-        <v>640.558</v>
-      </c>
-      <c r="D134" t="n">
-        <v>410.964</v>
-      </c>
+      <c r="C134" t="inlineStr"/>
+      <c r="D134" t="inlineStr"/>
       <c r="E134" t="n">
         <v>520.504</v>
       </c>
@@ -6280,12 +5364,8 @@
       <c r="B135" t="n">
         <v>497.48</v>
       </c>
-      <c r="C135" t="n">
-        <v>640.6079999999999</v>
-      </c>
-      <c r="D135" t="n">
-        <v>410.717</v>
-      </c>
+      <c r="C135" t="inlineStr"/>
+      <c r="D135" t="inlineStr"/>
       <c r="E135" t="n">
         <v>524.768</v>
       </c>
@@ -6315,12 +5395,8 @@
       <c r="B136" t="n">
         <v>491.907</v>
       </c>
-      <c r="C136" t="n">
-        <v>641.36</v>
-      </c>
-      <c r="D136" t="n">
-        <v>406.516</v>
-      </c>
+      <c r="C136" t="inlineStr"/>
+      <c r="D136" t="inlineStr"/>
       <c r="E136" t="n">
         <v>525.853</v>
       </c>
@@ -6350,12 +5426,8 @@
       <c r="B137" t="n">
         <v>488.854</v>
       </c>
-      <c r="C137" t="n">
-        <v>643.136</v>
-      </c>
-      <c r="D137" t="n">
-        <v>400.824</v>
-      </c>
+      <c r="C137" t="inlineStr"/>
+      <c r="D137" t="inlineStr"/>
       <c r="E137" t="n">
         <v>525.633</v>
       </c>
@@ -6385,12 +5457,8 @@
       <c r="B138" t="n">
         <v>487.426</v>
       </c>
-      <c r="C138" t="n">
-        <v>643.8630000000001</v>
-      </c>
-      <c r="D138" t="n">
-        <v>394.605</v>
-      </c>
+      <c r="C138" t="inlineStr"/>
+      <c r="D138" t="inlineStr"/>
       <c r="E138" t="n">
         <v>523.606</v>
       </c>
@@ -6420,12 +5488,8 @@
       <c r="B139" t="n">
         <v>482.379</v>
       </c>
-      <c r="C139" t="n">
-        <v>643.825</v>
-      </c>
-      <c r="D139" t="n">
-        <v>389.501</v>
-      </c>
+      <c r="C139" t="inlineStr"/>
+      <c r="D139" t="inlineStr"/>
       <c r="E139" t="n">
         <v>520.043</v>
       </c>
@@ -6455,12 +5519,8 @@
       <c r="B140" t="n">
         <v>477.264</v>
       </c>
-      <c r="C140" t="n">
-        <v>644.154</v>
-      </c>
-      <c r="D140" t="n">
-        <v>384.933</v>
-      </c>
+      <c r="C140" t="inlineStr"/>
+      <c r="D140" t="inlineStr"/>
       <c r="E140" t="n">
         <v>519.5410000000001</v>
       </c>
@@ -6490,12 +5550,8 @@
       <c r="B141" t="n">
         <v>474.892</v>
       </c>
-      <c r="C141" t="n">
-        <v>644.564</v>
-      </c>
-      <c r="D141" t="n">
-        <v>380.765</v>
-      </c>
+      <c r="C141" t="inlineStr"/>
+      <c r="D141" t="inlineStr"/>
       <c r="E141" t="n">
         <v>521.15</v>
       </c>
@@ -6525,12 +5581,8 @@
       <c r="B142" t="n">
         <v>471.286</v>
       </c>
-      <c r="C142" t="n">
-        <v>645.02</v>
-      </c>
-      <c r="D142" t="n">
-        <v>377.934</v>
-      </c>
+      <c r="C142" t="inlineStr"/>
+      <c r="D142" t="inlineStr"/>
       <c r="E142" t="inlineStr"/>
       <c r="F142" t="inlineStr"/>
       <c r="G142" t="inlineStr"/>
@@ -6556,12 +5608,8 @@
       <c r="B143" t="n">
         <v>471.286</v>
       </c>
-      <c r="C143" t="n">
-        <v>645.02</v>
-      </c>
-      <c r="D143" t="n">
-        <v>377.934</v>
-      </c>
+      <c r="C143" t="inlineStr"/>
+      <c r="D143" t="inlineStr"/>
       <c r="E143" t="inlineStr"/>
       <c r="F143" t="inlineStr"/>
       <c r="G143" t="inlineStr"/>
@@ -6587,12 +5635,8 @@
       <c r="B144" t="n">
         <v>462.796</v>
       </c>
-      <c r="C144" t="n">
-        <v>645.2670000000001</v>
-      </c>
-      <c r="D144" t="n">
-        <v>375.692</v>
-      </c>
+      <c r="C144" t="inlineStr"/>
+      <c r="D144" t="inlineStr"/>
       <c r="E144" t="inlineStr"/>
       <c r="F144" t="inlineStr"/>
       <c r="G144" t="inlineStr"/>
@@ -6618,12 +5662,8 @@
       <c r="B145" t="n">
         <v>460.551</v>
       </c>
-      <c r="C145" t="n">
-        <v>645.641</v>
-      </c>
-      <c r="D145" t="n">
-        <v>370.96</v>
-      </c>
+      <c r="C145" t="inlineStr"/>
+      <c r="D145" t="inlineStr"/>
       <c r="E145" t="inlineStr"/>
       <c r="F145" t="inlineStr"/>
       <c r="G145" t="inlineStr"/>
@@ -6649,12 +5689,8 @@
       <c r="B146" t="n">
         <v>457.618</v>
       </c>
-      <c r="C146" t="n">
-        <v>646.836</v>
-      </c>
-      <c r="D146" t="n">
-        <v>363.134</v>
-      </c>
+      <c r="C146" t="inlineStr"/>
+      <c r="D146" t="inlineStr"/>
       <c r="E146" t="inlineStr"/>
       <c r="F146" t="inlineStr"/>
       <c r="G146" t="inlineStr"/>
@@ -6680,12 +5716,8 @@
       <c r="B147" t="n">
         <v>453.911</v>
       </c>
-      <c r="C147" t="n">
-        <v>646.574</v>
-      </c>
-      <c r="D147" t="n">
-        <v>355.299</v>
-      </c>
+      <c r="C147" t="inlineStr"/>
+      <c r="D147" t="inlineStr"/>
       <c r="E147" t="inlineStr"/>
       <c r="F147" t="inlineStr"/>
       <c r="G147" t="inlineStr"/>
@@ -6711,12 +5743,8 @@
       <c r="B148" t="n">
         <v>449.581</v>
       </c>
-      <c r="C148" t="n">
-        <v>647.443</v>
-      </c>
-      <c r="D148" t="n">
-        <v>348.877</v>
-      </c>
+      <c r="C148" t="inlineStr"/>
+      <c r="D148" t="inlineStr"/>
       <c r="E148" t="inlineStr"/>
       <c r="F148" t="inlineStr"/>
       <c r="G148" t="inlineStr"/>
@@ -6742,12 +5770,8 @@
       <c r="B149" t="n">
         <v>447.25</v>
       </c>
-      <c r="C149" t="n">
-        <v>647.622</v>
-      </c>
-      <c r="D149" t="n">
-        <v>343.388</v>
-      </c>
+      <c r="C149" t="inlineStr"/>
+      <c r="D149" t="inlineStr"/>
       <c r="E149" t="inlineStr"/>
       <c r="F149" t="inlineStr"/>
       <c r="G149" t="inlineStr"/>
@@ -6773,12 +5797,8 @@
       <c r="B150" t="n">
         <v>442.507</v>
       </c>
-      <c r="C150" t="n">
-        <v>648.362</v>
-      </c>
-      <c r="D150" t="n">
-        <v>336.404</v>
-      </c>
+      <c r="C150" t="inlineStr"/>
+      <c r="D150" t="inlineStr"/>
       <c r="E150" t="inlineStr"/>
       <c r="F150" t="inlineStr"/>
       <c r="G150" t="inlineStr"/>
@@ -6804,12 +5824,8 @@
       <c r="B151" t="n">
         <v>437.052</v>
       </c>
-      <c r="C151" t="n">
-        <v>648.396</v>
-      </c>
-      <c r="D151" t="n">
-        <v>329.123</v>
-      </c>
+      <c r="C151" t="inlineStr"/>
+      <c r="D151" t="inlineStr"/>
       <c r="E151" t="inlineStr"/>
       <c r="F151" t="inlineStr"/>
       <c r="G151" t="inlineStr"/>
@@ -6835,12 +5851,8 @@
       <c r="B152" t="n">
         <v>434.829</v>
       </c>
-      <c r="C152" t="n">
-        <v>648.578</v>
-      </c>
-      <c r="D152" t="n">
-        <v>323.018</v>
-      </c>
+      <c r="C152" t="inlineStr"/>
+      <c r="D152" t="inlineStr"/>
       <c r="E152" t="inlineStr"/>
       <c r="F152" t="inlineStr"/>
       <c r="G152" t="inlineStr"/>
@@ -6866,12 +5878,8 @@
       <c r="B153" t="n">
         <v>433.142</v>
       </c>
-      <c r="C153" t="n">
-        <v>648.519</v>
-      </c>
-      <c r="D153" t="n">
-        <v>319.637</v>
-      </c>
+      <c r="C153" t="inlineStr"/>
+      <c r="D153" t="inlineStr"/>
       <c r="E153" t="inlineStr"/>
       <c r="F153" t="inlineStr"/>
       <c r="G153" t="inlineStr"/>
@@ -6897,12 +5905,8 @@
       <c r="B154" t="n">
         <v>429.692</v>
       </c>
-      <c r="C154" t="n">
-        <v>648.628</v>
-      </c>
-      <c r="D154" t="n">
-        <v>315.831</v>
-      </c>
+      <c r="C154" t="inlineStr"/>
+      <c r="D154" t="inlineStr"/>
       <c r="E154" t="n">
         <v>521.715</v>
       </c>
@@ -6911,12 +5915,8 @@
       </c>
       <c r="G154" t="inlineStr"/>
       <c r="H154" t="inlineStr"/>
-      <c r="I154" t="n">
-        <v>546.0890000000001</v>
-      </c>
-      <c r="J154" t="n">
-        <v>224.293</v>
-      </c>
+      <c r="I154" t="inlineStr"/>
+      <c r="J154" t="inlineStr"/>
       <c r="K154" t="inlineStr"/>
       <c r="L154" t="inlineStr"/>
       <c r="M154" t="n">
@@ -6936,12 +5936,8 @@
       <c r="B155" t="n">
         <v>427.843</v>
       </c>
-      <c r="C155" t="n">
-        <v>648.611</v>
-      </c>
-      <c r="D155" t="n">
-        <v>312.027</v>
-      </c>
+      <c r="C155" t="inlineStr"/>
+      <c r="D155" t="inlineStr"/>
       <c r="E155" t="n">
         <v>521.927</v>
       </c>

</xml_diff>